<commit_message>
some updates relating to string "CO2" -> subscript of 2
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98215770-3E01-48A1-A5C3-A3B9959122CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEA745-ED4B-4419-86B6-6E9D2D38E320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1279,7 +1279,7 @@
     <t>CO₂-Emissionen kantonaler Gebäude (Mietermodell) pro m2 (witterungsbereinigt)</t>
   </si>
   <si>
-    <t>t CO₂-Äquivalente (CO₂eq) pro Kopf</t>
+    <t>Tonnen CO₂-Äquivalente (CO₂eq) pro Kopf</t>
   </si>
 </sst>
 </file>
@@ -4842,7 +4842,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -7485,15 +7485,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7698,6 +7689,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
@@ -7710,14 +7710,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7734,4 +7726,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
IG3 und KV3: textliche Anpassung CO2
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEA745-ED4B-4419-86B6-6E9D2D38E320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75010DA6-B5EC-4D92-BD8B-C6D82DE874AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,9 +823,6 @@
     <t>durchschnittliches_GWP</t>
   </si>
   <si>
-    <t>CO₂-Äquivalente (CO₂eq)</t>
-  </si>
-  <si>
     <t>Durchschnittliche Treibhauswirkung (Global Warming Potential - GWP)</t>
   </si>
   <si>
@@ -1280,6 +1277,9 @@
   </si>
   <si>
     <t>Tonnen CO₂-Äquivalente (CO₂eq) pro Kopf</t>
+  </si>
+  <si>
+    <t>GWP in CO₂-Äquivalente (CO₂eq)</t>
   </si>
 </sst>
 </file>
@@ -4842,7 +4842,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U13" sqref="U13"/>
+      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -5674,10 +5674,10 @@
         <v>236</v>
       </c>
       <c r="U12" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>237</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>238</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5702,10 +5702,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>239</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>240</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
@@ -5714,13 +5714,13 @@
         <v>189</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>242</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>243</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5732,19 +5732,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>244</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>245</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25">
@@ -5755,10 +5755,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>247</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>248</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5770,7 +5770,7 @@
         <v>180</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5780,28 +5780,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>253</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>165</v>
@@ -5821,19 +5821,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>180</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5848,23 +5848,23 @@
         <v>226</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="U15" s="25" t="s">
+      <c r="V15" s="25" t="s">
         <v>259</v>
-      </c>
-      <c r="V15" s="25" t="s">
-        <v>260</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>165</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>186</v>
@@ -5881,22 +5881,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>387</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>388</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>180</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5905,17 +5905,17 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="U16" s="25" t="s">
+      <c r="V16" s="25" t="s">
         <v>266</v>
-      </c>
-      <c r="V16" s="25" t="s">
-        <v>267</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>165</v>
@@ -5938,19 +5938,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>180</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -5959,23 +5959,23 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>272</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>273</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>177</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="Y17" s="25" t="s">
-        <v>275</v>
       </c>
       <c r="AA17" s="25" t="s">
         <v>211</v>
@@ -5992,10 +5992,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>276</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>277</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
@@ -6016,20 +6016,20 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>279</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>280</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y18" s="25" t="s">
         <v>184</v>
@@ -6050,10 +6050,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
@@ -6077,31 +6077,31 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="W19" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="W19" s="35" t="s">
-        <v>285</v>
-      </c>
       <c r="X19" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y19" s="25" t="s">
         <v>184</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>186</v>
@@ -6118,7 +6118,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
@@ -6130,7 +6130,7 @@
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6139,7 +6139,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6148,13 +6148,13 @@
         <v>162</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6163,16 +6163,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>292</v>
-      </c>
-      <c r="X20" s="25" t="s">
-        <v>293</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25">
@@ -6186,7 +6186,7 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
@@ -6198,7 +6198,7 @@
         <v>180</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6210,14 +6210,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6245,7 +6245,7 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
@@ -6278,10 +6278,10 @@
         <v>226</v>
       </c>
       <c r="P22" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>300</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>301</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6290,10 +6290,10 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="W22" s="35" t="s">
         <v>302</v>
-      </c>
-      <c r="W22" s="35" t="s">
-        <v>303</v>
       </c>
       <c r="X22" s="25" t="s">
         <v>232</v>
@@ -6302,7 +6302,7 @@
         <v>184</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AA22" s="25" t="s">
         <v>186</v>
@@ -6316,10 +6316,10 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>305</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>306</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
@@ -6353,22 +6353,22 @@
         <v>226</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>307</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>308</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="V23" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="V23" s="25" t="s">
+      <c r="W23" s="35" t="s">
         <v>310</v>
-      </c>
-      <c r="W23" s="35" t="s">
-        <v>311</v>
       </c>
       <c r="X23" s="25" t="s">
         <v>232</v>
@@ -6377,7 +6377,7 @@
         <v>184</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA23" s="25" t="s">
         <v>186</v>
@@ -6394,10 +6394,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>313</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>314</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -6409,7 +6409,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6431,10 +6431,10 @@
         <v>226</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>316</v>
-      </c>
-      <c r="Q24" s="25" t="s">
-        <v>317</v>
       </c>
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
@@ -6443,10 +6443,10 @@
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="W24" s="35" t="s">
         <v>318</v>
-      </c>
-      <c r="W24" s="35" t="s">
-        <v>319</v>
       </c>
       <c r="X24" s="25" t="s">
         <v>232</v>
@@ -6455,7 +6455,7 @@
         <v>184</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA24" s="25" t="s">
         <v>186</v>
@@ -6472,10 +6472,10 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>320</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>321</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
@@ -6509,37 +6509,37 @@
         <v>226</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>323</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>324</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="W25" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="X25" s="25" t="s">
         <v>325</v>
-      </c>
-      <c r="W25" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="X25" s="25" t="s">
-        <v>326</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>184</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA25" s="25" t="s">
         <v>186</v>
@@ -6556,10 +6556,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>327</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>328</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
@@ -6593,37 +6593,37 @@
         <v>226</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>323</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>324</v>
       </c>
       <c r="S26" s="25">
         <v>300</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W26" s="35" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="X26" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>184</v>
       </c>
       <c r="Z26" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>186</v>
@@ -6640,22 +6640,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>333</v>
-      </c>
-      <c r="H27" t="s">
-        <v>334</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6665,14 +6665,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6680,29 +6680,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>337</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>338</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>165</v>
       </c>
       <c r="Z27" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="AA27" s="25" t="s">
         <v>340</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>341</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25">
@@ -6713,32 +6713,32 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>343</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>344</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>345</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>346</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
@@ -6747,7 +6747,7 @@
         <v>182</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6758,7 +6758,7 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
@@ -6775,7 +6775,7 @@
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25">
@@ -6786,7 +6786,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6818,7 +6818,7 @@
         <v>182</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6829,7 +6829,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6838,7 +6838,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6853,10 +6853,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6898,7 +6898,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6924,10 +6924,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>357</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>358</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
@@ -6939,7 +6939,7 @@
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6952,31 +6952,31 @@
         <v>191</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>362</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>363</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>364</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>165</v>
@@ -6990,25 +6990,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>365</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>366</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>332</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>333</v>
-      </c>
       <c r="H32" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7018,7 +7018,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7034,7 +7034,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>165</v>
@@ -7053,10 +7053,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>368</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>369</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7068,7 +7068,7 @@
         <v>180</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7080,16 +7080,16 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>165</v>
@@ -7103,35 +7103,35 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>346</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
@@ -7140,7 +7140,7 @@
         <v>182</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7151,7 +7151,7 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
@@ -7192,7 +7192,7 @@
         <v>180</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7209,11 +7209,11 @@
         <v>182</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7222,11 +7222,11 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Y35" s="25" t="s">
         <v>224</v>
@@ -7263,7 +7263,7 @@
         <v>180</v>
       </c>
       <c r="H36" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7275,16 +7275,16 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>165</v>
@@ -7298,13 +7298,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>155</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>157</v>
@@ -7319,7 +7319,7 @@
         <v>160</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7364,13 +7364,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>155</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>157</v>
@@ -7385,7 +7385,7 @@
         <v>160</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Neuer Indikator KV6: Anzahl Dieselbusse im ZVV
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75010DA6-B5EC-4D92-BD8B-C6D82DE874AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ADD344-6E59-451B-8357-03E03EB08162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="396">
   <si>
     <t>#</t>
   </si>
@@ -1280,6 +1280,24 @@
   </si>
   <si>
     <t>GWP in CO₂-Äquivalente (CO₂eq)</t>
+  </si>
+  <si>
+    <t>KV6</t>
+  </si>
+  <si>
+    <t>Anzahl Dieselbusse im ZVV</t>
+  </si>
+  <si>
+    <t>zvv</t>
+  </si>
+  <si>
+    <t>KV6_data.csv</t>
+  </si>
+  <si>
+    <t>Anzahl Dieselbusse</t>
+  </si>
+  <si>
+    <t>Zürcher Verkehrsverbund (ZVV)</t>
   </si>
 </sst>
 </file>
@@ -2707,7 +2725,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="6" customHeight="1"/>
-    <row r="4" spans="1:11" ht="101.25">
+    <row r="4" spans="1:11" ht="100.5">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -4836,13 +4854,13 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Z19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomRight" activeCell="AE39" sqref="AE39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -7424,6 +7442,56 @@
       <c r="AB38" s="25"/>
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
+    </row>
+    <row r="39" spans="1:31" ht="12" customHeight="1">
+      <c r="A39" s="25">
+        <v>0</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="G39" t="s">
+        <v>180</v>
+      </c>
+      <c r="H39" t="s">
+        <v>393</v>
+      </c>
+      <c r="J39" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39">
+        <v>2020</v>
+      </c>
+      <c r="O39" t="s">
+        <v>93</v>
+      </c>
+      <c r="U39" t="s">
+        <v>93</v>
+      </c>
+      <c r="V39" t="s">
+        <v>394</v>
+      </c>
+      <c r="X39" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD31">
@@ -7485,6 +7553,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7689,15 +7766,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
@@ -7710,6 +7778,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7726,12 +7802,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KV6: new indicator (script & data)
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5FB879-656F-45B8-AE9E-47C6EA7E9BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD06C32-D387-4890-A518-67DD3394EE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="397">
   <si>
     <t>#</t>
   </si>
@@ -1285,9 +1285,6 @@
     <t>KV6</t>
   </si>
   <si>
-    <t>Anzahl Dieselbusse im ZVV</t>
-  </si>
-  <si>
     <t>zvv</t>
   </si>
   <si>
@@ -1298,6 +1295,12 @@
   </si>
   <si>
     <t>Zürcher Verkehrsverbund (ZVV)</t>
+  </si>
+  <si>
+    <t>Anzahl Dieselbusse im Zürcher Verkehrsverbund (ZVV)</t>
+  </si>
+  <si>
+    <t>Anzahl Dieselbusse ZVV</t>
   </si>
 </sst>
 </file>
@@ -4857,10 +4860,10 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Z19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -7451,22 +7454,22 @@
         <v>390</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G39" t="s">
         <v>180</v>
       </c>
       <c r="H39" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7481,10 +7484,10 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>393</v>
+      </c>
+      <c r="X39" t="s">
         <v>394</v>
-      </c>
-      <c r="X39" t="s">
-        <v>395</v>
       </c>
       <c r="Y39" t="s">
         <v>165</v>
@@ -7553,6 +7556,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7757,15 +7769,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
@@ -7778,6 +7781,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7794,12 +7805,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
switch input dataset_name indicator_name
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD06C32-D387-4890-A518-67DD3394EE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CFBF95-7086-483E-8064-EE56905A2DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2237,6 +2237,33 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2346,33 +2373,6 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="90" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2421,38 +2421,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Über112" displayName="Über112" ref="A4:K50" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Über112" displayName="Über112" ref="A4:K50" totalsRowCount="1" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A4:K49" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Titel" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Titel" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula array="1">HYPERLINK("" &amp; "#" &amp; A5 &amp; "!B5",INDIRECT("'" &amp; $A5 &amp; "'!B5"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mehrinvestitionen" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mehrinvestitionen" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B13")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Jährliche Mehrkosten " dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Jährliche Mehrkosten " dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B14")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Personal" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Personal" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B15")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="MI: Unterer Wert" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="MI: Unterer Wert" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Mehrinvestitionen]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MI: oberer Wert" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MI: oberer Wert" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Mehrinvestitionen]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="MK: Unterer Wert" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="MK: Unterer Wert" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Jährliche Mehrkosten ]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MK: Oberer Wert" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MK: Oberer Wert" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Jährliche Mehrkosten ]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="P: Unterer Wert" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="P: Unterer Wert" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Personal]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="P: Oberer Wert" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="P: Oberer Wert" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Personal]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4834,13 +4834,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A5:A17 A19 A21 A23 A25 A27 A29 A31">
-    <cfRule type="duplicateValues" dxfId="26" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 A20 A22 A24 A26 A28 A30">
-    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:E31">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"tbd"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4863,7 +4863,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -7454,10 +7454,10 @@
         <v>390</v>
       </c>
       <c r="C39" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>395</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>396</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
@@ -7556,15 +7556,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7769,6 +7760,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
@@ -7781,14 +7781,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7805,4 +7797,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
EV3: Update INDICATOR_NAME. Required adjustment in Monitoring XLSX.
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B105PCG\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CFBF95-7086-483E-8064-EE56905A2DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -33,16 +32,16 @@
     <definedName name="Ü5">#REF!</definedName>
     <definedName name="Ü6">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -61,26 +60,42 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={8D6D4BDD-30EE-4AB7-91B4-A0AFA8CAA1BF}</author>
     <author>tc={F8D71A7C-E5F7-4AB2-BA3A-263385823BB9}</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Arial Nova Cond"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Titel der Grafiken</t>
+        </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="K20" authorId="1" shapeId="0">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color theme="1"/>
+            <rFont val="Arial Nova Cond"/>
+            <family val="2"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Jährliche Daten erst seit 1996 verfügbar, deshalb dort Start auch wenn erste Daten aus 1975 stammen.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -88,14 +103,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -646,9 +661,6 @@
     <t>Strom</t>
   </si>
   <si>
-    <t>Gesamtstromverbrauch nach Energieträger</t>
-  </si>
-  <si>
     <t>awel</t>
   </si>
   <si>
@@ -1301,12 +1313,15 @@
   </si>
   <si>
     <t>Anzahl Dieselbusse ZVV</t>
+  </si>
+  <si>
+    <t>Gesamtstromverbrauch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;CHF&quot;_-;\-* #,##0.00\ &quot;CHF&quot;_-;_-* &quot;-&quot;??\ &quot;CHF&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;CHF&quot;_-;\-* #,##0\ &quot;CHF&quot;_-;_-* &quot;-&quot;??\ &quot;CHF&quot;_-;_-@_-"/>
@@ -2166,32 +2181,32 @@
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="20 % - Akzent1" xfId="42" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent1 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20 % - Akzent1 2" xfId="7"/>
     <cellStyle name="20 % - Akzent2" xfId="45" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="49" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent4" xfId="52" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20 % - Akzent4 2" xfId="6"/>
     <cellStyle name="20 % - Akzent5" xfId="56" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent6" xfId="60" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent1" xfId="43" builtinId="31" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent2" xfId="46" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent3" xfId="2" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3 2" xfId="67" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40 % - Akzent3 2" xfId="67"/>
     <cellStyle name="40 % - Akzent4" xfId="53" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent5" xfId="57" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent6" xfId="61" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent1" xfId="44" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60 % - Akzent1 2" xfId="5"/>
     <cellStyle name="60 % - Akzent2" xfId="47" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent3" xfId="50" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent4" xfId="54" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent5" xfId="58" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent6" xfId="62" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent Gelb" xfId="21" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Akzent Gelb" xfId="21"/>
     <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent1 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Akzent1 2" xfId="3"/>
     <cellStyle name="Akzent2" xfId="1" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Akzent2 2" xfId="66"/>
     <cellStyle name="Akzent3" xfId="48" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Akzent4" xfId="51" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Akzent5" xfId="55" builtinId="45" customBuiltin="1"/>
@@ -2200,69 +2215,42 @@
     <cellStyle name="Berechnung" xfId="36" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Eingabe" xfId="19" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Eingabe 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Eingabe 2" xfId="64"/>
     <cellStyle name="Ergebnis" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="40" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gelb hell" xfId="22" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="grau" xfId="20" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Gelb hell" xfId="22"/>
+    <cellStyle name="grau" xfId="20"/>
     <cellStyle name="Gut" xfId="32" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Gut 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Hyperlink" xfId="68" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Lien hypertexte 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Gut 2" xfId="16"/>
+    <cellStyle name="Hyperlink" xfId="68"/>
+    <cellStyle name="Lien hypertexte 2" xfId="25"/>
     <cellStyle name="Link" xfId="8" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Link 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Link 2" xfId="24"/>
     <cellStyle name="Neutral" xfId="34" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal_Gewichtung Übergang EVE-LIK (V.2)" xfId="26" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Notiz 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal_Gewichtung Übergang EVE-LIK (V.2)" xfId="26"/>
+    <cellStyle name="Notiz 2" xfId="65"/>
     <cellStyle name="Prozent" xfId="10" builtinId="5"/>
     <cellStyle name="Schlecht" xfId="33" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Schlecht 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Schlecht 2" xfId="15"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Standard 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Standard 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Standard 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Standard 4" xfId="63" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Standard 4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Standard 2" xfId="4"/>
+    <cellStyle name="Standard 2 2" xfId="12"/>
+    <cellStyle name="Standard 3" xfId="23"/>
+    <cellStyle name="Standard 4" xfId="63"/>
+    <cellStyle name="Standard 4 2" xfId="17"/>
     <cellStyle name="Überschrift" xfId="27" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="28" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="29" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="30" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 4" xfId="31" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Überschrift 5" xfId="11" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Überschrift 4 2" xfId="13"/>
+    <cellStyle name="Überschrift 5" xfId="11"/>
     <cellStyle name="Verknüpfte Zelle" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Währung 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Währung 2" xfId="14"/>
     <cellStyle name="Warnender Text" xfId="39" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="38" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2373,6 +2361,33 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="90" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2421,38 +2436,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Über112" displayName="Über112" ref="A4:K50" totalsRowCount="1" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A4:K49" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Über112" displayName="Über112" ref="A4:K50" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A4:K49"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Titel" dataDxfId="22" totalsRowDxfId="21">
+    <tableColumn id="1" name="#" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" name="Titel" dataDxfId="19" totalsRowDxfId="18">
       <calculatedColumnFormula array="1">HYPERLINK("" &amp; "#" &amp; A5 &amp; "!B5",INDIRECT("'" &amp; $A5 &amp; "'!B5"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Mehrinvestitionen" dataDxfId="20" totalsRowDxfId="19">
+    <tableColumn id="8" name="Mehrinvestitionen" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B13")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Jährliche Mehrkosten " dataDxfId="18" totalsRowDxfId="17">
+    <tableColumn id="9" name="Jährliche Mehrkosten " dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B14")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Personal" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="12" name="Personal" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula array="1">INDIRECT("'" &amp; A5 &amp; "'!B15")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="MI: Unterer Wert" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="16" name="MI: Unterer Wert" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Mehrinvestitionen]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MI: oberer Wert" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="17" name="MI: oberer Wert" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Mehrinvestitionen]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="MK: Unterer Wert" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="18" name="MK: Unterer Wert" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Jährliche Mehrkosten ]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MK: Oberer Wert" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="19" name="MK: Oberer Wert" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Jährliche Mehrkosten ]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="P: Unterer Wert" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="20" name="P: Unterer Wert" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Personal]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="P: Oberer Wert" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
+    <tableColumn id="21" name="P: Oberer Wert" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>IFERROR(_xlfn.XLOOKUP(Über112[[#This Row],[Personal]],#REF!,#REF!,#N/A),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2697,7 +2712,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1">
     <tabColor theme="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -4834,13 +4849,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A5:A17 A19 A21 A23 A25 A27 A29 A31">
-    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18 A20 A22 A24 A26 A28 A30">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:E31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"tbd"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4853,17 +4868,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1"/>
@@ -5191,19 +5206,19 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>178</v>
+        <v>396</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="H5" s="25" t="s">
         <v>180</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>181</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>86</v>
@@ -5213,13 +5228,13 @@
       </c>
       <c r="L5" s="25"/>
       <c r="N5" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O5" s="25" t="s">
         <v>177</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
@@ -5235,13 +5250,13 @@
         <v>101</v>
       </c>
       <c r="Y5" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z5" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="AA5" s="25" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="14.25">
@@ -5252,22 +5267,22 @@
         <v>53</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>188</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25" t="s">
@@ -5277,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M6" s="25">
         <v>8100.01</v>
@@ -5286,37 +5301,37 @@
         <v>162</v>
       </c>
       <c r="O6" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="P6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="Q6" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>194</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="V6" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="V6" s="25" t="s">
+      <c r="W6" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="W6" s="25" t="s">
+      <c r="X6" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="Y6" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z6" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="Y6" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z6" s="32" t="s">
-        <v>199</v>
-      </c>
       <c r="AA6" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
@@ -5333,19 +5348,19 @@
         <v>89</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H7" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>86</v>
@@ -5356,13 +5371,13 @@
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
       <c r="N7" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>182</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
@@ -5381,10 +5396,10 @@
         <v>165</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1">
@@ -5398,7 +5413,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
@@ -5407,47 +5422,47 @@
         <v>169</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>205</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>206</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
       </c>
       <c r="L8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>208</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>209</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="14.25">
@@ -5461,19 +5476,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>214</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>215</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5484,12 +5499,12 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5502,14 +5517,14 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>165</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
@@ -5523,22 +5538,22 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>218</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>219</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H10" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5549,34 +5564,34 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
@@ -5593,13 +5608,13 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>104</v>
@@ -5614,7 +5629,7 @@
         <v>2005</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M11" s="25">
         <v>0.1</v>
@@ -5623,34 +5638,34 @@
         <v>162</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="V11" s="25" t="s">
+      <c r="W11" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="X11" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="X11" s="25" t="s">
+      <c r="Y11" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z11" s="25" t="s">
         <v>232</v>
       </c>
-      <c r="Y11" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>233</v>
-      </c>
       <c r="AA11" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25">
@@ -5664,19 +5679,19 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5685,20 +5700,20 @@
         <v>2020</v>
       </c>
       <c r="N12" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="U12" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>236</v>
-      </c>
-      <c r="U12" s="25" t="s">
-        <v>389</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>237</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5709,7 +5724,7 @@
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -5723,25 +5738,25 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>238</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>239</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>241</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>242</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5753,19 +5768,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>243</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>244</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25">
@@ -5776,22 +5791,22 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>246</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>247</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H14" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5801,28 +5816,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>252</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>165</v>
@@ -5842,19 +5857,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>255</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>256</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5863,32 +5878,32 @@
         <v>2021</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="U15" s="25" t="s">
+      <c r="V15" s="25" t="s">
         <v>258</v>
-      </c>
-      <c r="V15" s="25" t="s">
-        <v>259</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>165</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA15" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB15"/>
       <c r="AC15"/>
@@ -5902,22 +5917,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>386</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>387</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>263</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5926,23 +5941,23 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="U16" s="25" t="s">
+      <c r="V16" s="25" t="s">
         <v>265</v>
-      </c>
-      <c r="V16" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -5959,19 +5974,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -5980,26 +5995,26 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>271</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>272</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>177</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="Y17" s="25" t="s">
-        <v>274</v>
-      </c>
       <c r="AA17" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -6013,19 +6028,19 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>275</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F18" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="34" t="s">
         <v>179</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>180</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>122</v>
@@ -6037,27 +6052,27 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>278</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>336</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>279</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Y18" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z18"/>
       <c r="AA18" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB18"/>
       <c r="AC18"/>
@@ -6071,19 +6086,19 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>179</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>180</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>123</v>
@@ -6098,34 +6113,34 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="W19" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="W19" s="35" t="s">
+      <c r="X19" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y19" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z19" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="X19" s="25" t="s">
-        <v>280</v>
-      </c>
-      <c r="Y19" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z19" s="25" t="s">
-        <v>285</v>
-      </c>
       <c r="AA19" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="14.25">
@@ -6139,19 +6154,19 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6160,7 +6175,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6169,13 +6184,13 @@
         <v>162</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6184,16 +6199,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>291</v>
-      </c>
-      <c r="X20" s="25" t="s">
-        <v>292</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25">
@@ -6207,19 +6222,19 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F21" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H21" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6231,14 +6246,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6249,7 +6264,7 @@
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
@@ -6266,13 +6281,13 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>104</v>
@@ -6287,7 +6302,7 @@
         <v>2005</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M22">
         <v>0.1</v>
@@ -6296,13 +6311,13 @@
         <v>162</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P22" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>299</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>300</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6311,22 +6326,22 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="W22" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="W22" s="35" t="s">
+      <c r="X22" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y22" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z22" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="X22" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z22" s="25" t="s">
-        <v>303</v>
-      </c>
       <c r="AA22" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="14.25">
@@ -6337,16 +6352,16 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>304</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>305</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>104</v>
@@ -6362,7 +6377,7 @@
         <v>2005</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M23" s="25">
         <v>0.1</v>
@@ -6371,37 +6386,37 @@
         <v>162</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>306</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>307</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="V23" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="V23" s="25" t="s">
+      <c r="W23" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="W23" s="35" t="s">
+      <c r="X23" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y23" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z23" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="X23" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="Y23" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z23" s="25" t="s">
-        <v>311</v>
-      </c>
       <c r="AA23" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB23" s="25"/>
       <c r="AC23" s="25"/>
@@ -6415,22 +6430,22 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>312</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>313</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6440,7 +6455,7 @@
         <v>2005</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M24" s="25">
         <v>0.1</v>
@@ -6449,13 +6464,13 @@
         <v>162</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>315</v>
-      </c>
-      <c r="Q24" s="25" t="s">
-        <v>316</v>
       </c>
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
@@ -6464,22 +6479,22 @@
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="W24" s="35" t="s">
         <v>317</v>
       </c>
-      <c r="W24" s="35" t="s">
-        <v>318</v>
-      </c>
       <c r="X24" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y24" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB24" s="25"/>
       <c r="AC24" s="25"/>
@@ -6493,16 +6508,16 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>104</v>
@@ -6518,7 +6533,7 @@
         <v>2005</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M25" s="25">
         <v>0.1</v>
@@ -6527,43 +6542,43 @@
         <v>162</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>322</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>323</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="W25" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="X25" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="W25" s="35" t="s">
+      <c r="Y25" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z25" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="X25" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z25" s="25" t="s">
-        <v>311</v>
-      </c>
       <c r="AA25" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB25" s="25"/>
       <c r="AC25" s="25"/>
@@ -6577,16 +6592,16 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>326</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>327</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>104</v>
@@ -6602,7 +6617,7 @@
         <v>2005</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M26" s="25">
         <v>0.1</v>
@@ -6611,43 +6626,43 @@
         <v>162</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>322</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>323</v>
       </c>
       <c r="S26" s="25">
         <v>300</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W26" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="X26" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="Y26" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="X26" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z26" s="25" t="s">
-        <v>311</v>
-      </c>
       <c r="AA26" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AB26" s="25"/>
       <c r="AC26" s="25"/>
@@ -6661,22 +6676,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>332</v>
-      </c>
-      <c r="H27" t="s">
-        <v>333</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6686,14 +6701,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6701,29 +6716,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>336</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>165</v>
       </c>
       <c r="Z27" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="AA27" s="25" t="s">
         <v>339</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>340</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25">
@@ -6734,41 +6749,41 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>342</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>343</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>344</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>345</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6779,24 +6794,24 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25">
@@ -6807,7 +6822,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6832,14 +6847,14 @@
         <v>2002</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6850,7 +6865,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6859,7 +6874,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6874,10 +6889,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6901,16 +6916,16 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O30" s="25" t="s">
         <v>172</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6919,7 +6934,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6945,22 +6960,22 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>356</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>357</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6970,40 +6985,40 @@
         <v>2010</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>162</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>361</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>362</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>363</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15">
@@ -7011,25 +7026,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>364</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>365</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>332</v>
-      </c>
       <c r="H32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7039,7 +7054,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7055,7 +7070,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>165</v>
@@ -7074,22 +7089,22 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>367</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>368</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F33" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H33" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7101,22 +7116,22 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25">
@@ -7124,44 +7139,44 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>345</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7172,18 +7187,18 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
@@ -7207,13 +7222,13 @@
         <v>91</v>
       </c>
       <c r="F35" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H35" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7223,18 +7238,18 @@
         <v>2016</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M35" s="25"/>
       <c r="N35" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7243,18 +7258,18 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
@@ -7278,13 +7293,13 @@
         <v>91</v>
       </c>
       <c r="F36" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>180</v>
-      </c>
       <c r="H36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7296,22 +7311,22 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>165</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="14.25">
@@ -7319,13 +7334,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>155</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>157</v>
@@ -7340,7 +7355,7 @@
         <v>160</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7385,13 +7400,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>155</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>157</v>
@@ -7406,7 +7421,7 @@
         <v>160</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7451,25 +7466,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="G39" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" t="s">
         <v>391</v>
-      </c>
-      <c r="G39" t="s">
-        <v>180</v>
-      </c>
-      <c r="H39" t="s">
-        <v>392</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7484,59 +7499,59 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>392</v>
+      </c>
+      <c r="X39" t="s">
         <v>393</v>
-      </c>
-      <c r="X39" t="s">
-        <v>394</v>
       </c>
       <c r="Y39" t="s">
         <v>165</v>
       </c>
       <c r="AA39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD31">
+  <sortState ref="A2:AD31">
     <sortCondition ref="B2:B31"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G30" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="G23" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="G25" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="G26" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="G27" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="G28" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="G29" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="G24" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="G22" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="G20" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="G3" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="G4" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="G10" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="G8" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="G5" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="G7" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="G21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="G12" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="G15" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="G6" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="G9" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="G16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="G17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G18" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="G19" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="G32" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G31" r:id="rId1"/>
+    <hyperlink ref="G30" r:id="rId2"/>
+    <hyperlink ref="G23" r:id="rId3"/>
+    <hyperlink ref="G25" r:id="rId4"/>
+    <hyperlink ref="G26" r:id="rId5"/>
+    <hyperlink ref="G27" r:id="rId6"/>
+    <hyperlink ref="G28" r:id="rId7"/>
+    <hyperlink ref="G29" r:id="rId8"/>
+    <hyperlink ref="G24" r:id="rId9"/>
+    <hyperlink ref="G11" r:id="rId10"/>
+    <hyperlink ref="G22" r:id="rId11"/>
+    <hyperlink ref="G20" r:id="rId12"/>
+    <hyperlink ref="G3" r:id="rId13"/>
+    <hyperlink ref="G4" r:id="rId14"/>
+    <hyperlink ref="G10" r:id="rId15"/>
+    <hyperlink ref="G8" r:id="rId16"/>
+    <hyperlink ref="G5" r:id="rId17"/>
+    <hyperlink ref="G7" r:id="rId18"/>
+    <hyperlink ref="G21" r:id="rId19"/>
+    <hyperlink ref="G12" r:id="rId20"/>
+    <hyperlink ref="G15" r:id="rId21"/>
+    <hyperlink ref="G6" r:id="rId22"/>
+    <hyperlink ref="G9" r:id="rId23"/>
+    <hyperlink ref="G16" r:id="rId24"/>
+    <hyperlink ref="G17" r:id="rId25"/>
+    <hyperlink ref="G18" r:id="rId26"/>
+    <hyperlink ref="G19" r:id="rId27"/>
+    <hyperlink ref="G32" r:id="rId28"/>
+    <hyperlink ref="G33" r:id="rId29"/>
+    <hyperlink ref="G14" r:id="rId30"/>
+    <hyperlink ref="G34" r:id="rId31"/>
+    <hyperlink ref="G2" r:id="rId32"/>
+    <hyperlink ref="G35" r:id="rId33"/>
+    <hyperlink ref="G36" r:id="rId34"/>
+    <hyperlink ref="G37" r:id="rId35"/>
+    <hyperlink ref="G38" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
@@ -7545,14 +7560,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7761,21 +7774,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7800,9 +7812,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KV3: updated with data 2022, script adapted
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56858A27-C729-4214-8D1B-8519B1385E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A622B30B-B5E2-42C8-BB06-BFDCFC403D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-1488" windowWidth="23256" windowHeight="14016" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -487,9 +487,6 @@
     <t>Stromerzeugung mit Photovoltaik auf kantonalen Gebäuden</t>
   </si>
   <si>
-    <t>KV3_data.csv</t>
-  </si>
-  <si>
     <t>KV4_data.csv</t>
   </si>
   <si>
@@ -1313,6 +1310,9 @@
   </si>
   <si>
     <t>Pro-Kopf-Konsum von Fleisch gemäss Haushaltsbudgeterhebung (BFS)</t>
+  </si>
+  <si>
+    <t>KTZH_00002102_00004163.csv</t>
   </si>
 </sst>
 </file>
@@ -4876,10 +4876,10 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4914,97 +4914,97 @@
   <sheetData>
     <row r="1" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="K1" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="L1" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="X1" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="Y1" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Z1" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AA1" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AB1" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AC1" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AE1" t="s">
         <v>153</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5015,25 +5015,25 @@
         <v>68</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>160</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>161</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>86</v>
@@ -5044,7 +5044,7 @@
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
@@ -5056,24 +5056,24 @@
         <v>108</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W2" s="25"/>
       <c r="X2" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y2" s="25" t="s">
         <v>164</v>
-      </c>
-      <c r="Y2" s="25" t="s">
-        <v>165</v>
       </c>
       <c r="Z2" s="25"/>
       <c r="AA2" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AB2" s="25"/>
       <c r="AC2" s="25"/>
       <c r="AD2" s="25"/>
       <c r="AE2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5087,19 +5087,19 @@
         <v>114</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="25" t="s">
         <v>170</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>171</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>86</v>
@@ -5111,11 +5111,11 @@
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P3" s="25"/>
       <c r="Q3" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
@@ -5124,16 +5124,16 @@
         <v>115</v>
       </c>
       <c r="V3" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X3" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y3" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA3" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5147,19 +5147,19 @@
         <v>116</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>170</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>171</v>
       </c>
       <c r="J4" s="25" t="s">
         <v>86</v>
@@ -5171,11 +5171,11 @@
       <c r="M4" s="25"/>
       <c r="N4" s="25"/>
       <c r="O4" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P4" s="25"/>
       <c r="Q4" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R4" s="25"/>
       <c r="S4" s="25"/>
@@ -5184,16 +5184,16 @@
         <v>115</v>
       </c>
       <c r="V4" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X4" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y4" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA4" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5207,19 +5207,19 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="H5" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>180</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>86</v>
@@ -5229,13 +5229,13 @@
       </c>
       <c r="L5" s="25"/>
       <c r="N5" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q5" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="O5" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
@@ -5244,20 +5244,20 @@
         <v>115</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W5" s="25"/>
       <c r="X5" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y5" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z5" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>184</v>
-      </c>
-      <c r="AA5" s="25" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5268,22 +5268,22 @@
         <v>53</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>186</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>187</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25" t="s">
@@ -5293,46 +5293,46 @@
         <v>2021</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M6" s="25">
         <v>0.1</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P6" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q6" s="25" t="s">
         <v>392</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>393</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="V6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="V6" s="25" t="s">
+      <c r="W6" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="W6" s="25" t="s">
+      <c r="X6" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="Y6" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z6" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="Y6" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z6" s="32" t="s">
-        <v>196</v>
-      </c>
       <c r="AA6" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
@@ -5349,19 +5349,19 @@
         <v>89</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H7" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>86</v>
@@ -5372,13 +5372,13 @@
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
       <c r="N7" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
@@ -5387,20 +5387,20 @@
         <v>115</v>
       </c>
       <c r="V7" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W7" s="25"/>
       <c r="X7" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y7" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5414,56 +5414,56 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>203</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
       </c>
       <c r="L8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>205</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>206</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5477,19 +5477,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>211</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>212</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5500,12 +5500,12 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5518,14 +5518,14 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y9" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
@@ -5539,22 +5539,22 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>215</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>216</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H10" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5565,34 +5565,34 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
@@ -5609,13 +5609,13 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>104</v>
@@ -5630,43 +5630,43 @@
         <v>2005</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M11" s="25">
         <v>0.1</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="V11" s="25" t="s">
+      <c r="W11" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="X11" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="X11" s="25" t="s">
+      <c r="Y11" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z11" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="Y11" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>230</v>
-      </c>
       <c r="AA11" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5680,19 +5680,19 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G12" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5701,31 +5701,31 @@
         <v>2020</v>
       </c>
       <c r="N12" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="U12" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>233</v>
-      </c>
-      <c r="U12" s="25" t="s">
-        <v>383</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>234</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y12" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -5739,25 +5739,25 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>235</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>236</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>238</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>239</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5769,19 +5769,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="X13" s="25" t="s">
+      <c r="Y13" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA13" s="25" t="s">
         <v>241</v>
-      </c>
-      <c r="Y13" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="AA13" s="25" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5792,22 +5792,22 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H14" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5817,31 +5817,31 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>249</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y14" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB14"/>
       <c r="AC14"/>
@@ -5858,19 +5858,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>252</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>253</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5879,32 +5879,32 @@
         <v>2021</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="U15" s="25" t="s">
+      <c r="V15" s="25" t="s">
         <v>255</v>
-      </c>
-      <c r="V15" s="25" t="s">
-        <v>256</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y15" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z15" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="Y15" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z15" s="25" t="s">
-        <v>258</v>
-      </c>
       <c r="AA15" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB15"/>
       <c r="AC15"/>
@@ -5918,22 +5918,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>380</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>381</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>259</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>260</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5942,23 +5942,23 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="U16" s="25" t="s">
+      <c r="V16" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="V16" s="25" t="s">
-        <v>263</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y16" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -5975,19 +5975,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -5996,26 +5996,26 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="U17" s="25" t="s">
-        <v>269</v>
-      </c>
       <c r="V17" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="Y17" s="25" t="s">
-        <v>271</v>
-      </c>
       <c r="AA17" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -6029,22 +6029,22 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>272</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>273</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>169</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>122</v>
+        <v>397</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6053,27 +6053,27 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>274</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>275</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y18" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z18"/>
       <c r="AA18" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB18"/>
       <c r="AC18"/>
@@ -6087,22 +6087,22 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="G19" s="33" t="s">
-        <v>179</v>
-      </c>
       <c r="H19" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6114,34 +6114,34 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="W19" s="35" t="s">
         <v>280</v>
       </c>
-      <c r="W19" s="35" t="s">
+      <c r="X19" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y19" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z19" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="X19" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="Y19" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z19" s="25" t="s">
-        <v>282</v>
-      </c>
       <c r="AA19" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6155,19 +6155,19 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6176,22 +6176,22 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6200,16 +6200,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="X20" s="25" t="s">
+      <c r="Y20" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA20" s="25" t="s">
         <v>289</v>
-      </c>
-      <c r="Y20" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="AA20" s="25" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6223,19 +6223,19 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F21" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G21" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H21" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6247,25 +6247,25 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y21" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
@@ -6282,13 +6282,13 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>104</v>
@@ -6303,22 +6303,22 @@
         <v>2005</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M22" s="25">
         <v>0.1</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P22" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>296</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>297</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6327,22 +6327,22 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="W22" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="W22" s="35" t="s">
+      <c r="X22" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y22" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z22" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="X22" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z22" s="25" t="s">
-        <v>300</v>
-      </c>
       <c r="AA22" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6353,16 +6353,16 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>301</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>302</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>104</v>
@@ -6378,46 +6378,46 @@
         <v>2005</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M23" s="25">
         <v>0.1</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>303</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>304</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="V23" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="V23" s="25" t="s">
+      <c r="W23" s="35" t="s">
         <v>306</v>
       </c>
-      <c r="W23" s="35" t="s">
+      <c r="X23" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y23" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z23" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="X23" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y23" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z23" s="25" t="s">
-        <v>308</v>
-      </c>
       <c r="AA23" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB23" s="25"/>
       <c r="AC23" s="25"/>
@@ -6431,22 +6431,22 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>309</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>310</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6456,22 +6456,22 @@
         <v>2005</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M24" s="25">
         <v>0.1</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>312</v>
-      </c>
-      <c r="Q24" s="25" t="s">
-        <v>313</v>
       </c>
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
@@ -6480,22 +6480,22 @@
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="W24" s="35" t="s">
         <v>314</v>
       </c>
-      <c r="W24" s="35" t="s">
-        <v>315</v>
-      </c>
       <c r="X24" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Y24" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB24" s="25"/>
       <c r="AC24" s="25"/>
@@ -6509,16 +6509,16 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>316</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>317</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>104</v>
@@ -6534,52 +6534,52 @@
         <v>2005</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M25" s="25">
         <v>0.1</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="W25" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="X25" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="W25" s="35" t="s">
+      <c r="Y25" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z25" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="X25" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z25" s="25" t="s">
-        <v>308</v>
-      </c>
       <c r="AA25" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB25" s="25"/>
       <c r="AC25" s="25"/>
@@ -6593,16 +6593,16 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>323</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>324</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>104</v>
@@ -6618,52 +6618,52 @@
         <v>2005</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M26" s="25">
         <v>0.1</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="S26" s="25">
         <v>300</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="W26" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="X26" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y26" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="X26" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z26" s="25" t="s">
-        <v>308</v>
-      </c>
       <c r="AA26" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB26" s="25"/>
       <c r="AC26" s="25"/>
@@ -6677,22 +6677,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>329</v>
-      </c>
-      <c r="H27" t="s">
-        <v>330</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6702,14 +6702,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6717,29 +6717,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>333</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>334</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y27" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z27" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="Y27" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z27" s="25" t="s">
+      <c r="AA27" s="25" t="s">
         <v>336</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6750,41 +6750,41 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>339</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>340</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>341</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>342</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6795,24 +6795,24 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6823,7 +6823,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6832,10 +6832,10 @@
         <v>88</v>
       </c>
       <c r="F29" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" s="34" t="s">
         <v>169</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>170</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>99</v>
@@ -6848,14 +6848,14 @@
         <v>2002</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6866,7 +6866,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6875,7 +6875,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6890,19 +6890,19 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F30" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="25" t="s">
         <v>169</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>170</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>102</v>
@@ -6917,16 +6917,16 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O30" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6935,18 +6935,18 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y30" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z30" s="25"/>
       <c r="AA30" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AB30" s="25"/>
       <c r="AC30" s="25"/>
@@ -6961,22 +6961,22 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>353</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>354</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6986,40 +6986,40 @@
         <v>2010</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M31" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="O31" s="25" t="s">
         <v>395</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="O31" s="25" t="s">
-        <v>396</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>355</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>356</v>
       </c>
-      <c r="X31" s="25" t="s">
-        <v>357</v>
-      </c>
       <c r="Y31" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -7027,25 +7027,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>358</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>359</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>329</v>
-      </c>
       <c r="H32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7055,11 +7055,11 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O32" s="25"/>
       <c r="P32" s="30"/>
@@ -7071,10 +7071,10 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Y32" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Z32" s="25"/>
       <c r="AA32" s="25"/>
@@ -7090,22 +7090,22 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>361</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>362</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F33" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H33" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7117,22 +7117,22 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Y33" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -7140,44 +7140,44 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>342</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7188,18 +7188,18 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
@@ -7223,13 +7223,13 @@
         <v>91</v>
       </c>
       <c r="F35" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H35" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7239,18 +7239,18 @@
         <v>2016</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M35" s="25"/>
       <c r="N35" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7259,18 +7259,18 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
@@ -7294,13 +7294,13 @@
         <v>91</v>
       </c>
       <c r="F36" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>179</v>
-      </c>
       <c r="H36" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7312,22 +7312,22 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Y36" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -7335,28 +7335,28 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="25" t="s">
         <v>374</v>
       </c>
-      <c r="C37" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="D37" s="25" t="s">
+      <c r="E37" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="25" t="s">
         <v>375</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="I37" s="25" t="s">
-        <v>376</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7367,7 +7367,7 @@
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
       <c r="N37" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O37" s="25"/>
       <c r="P37" s="25"/>
@@ -7379,18 +7379,18 @@
         <v>115</v>
       </c>
       <c r="V37" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W37" s="25"/>
       <c r="X37" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y37" s="25" t="s">
         <v>164</v>
-      </c>
-      <c r="Y37" s="25" t="s">
-        <v>165</v>
       </c>
       <c r="Z37" s="25"/>
       <c r="AA37" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AB37" s="25"/>
       <c r="AC37" s="25"/>
@@ -7401,28 +7401,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="25" t="s">
         <v>377</v>
       </c>
-      <c r="C38" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" s="25" t="s">
+      <c r="E38" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="I38" s="25" t="s">
         <v>378</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>379</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7433,7 +7433,7 @@
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
       <c r="N38" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O38" s="25"/>
       <c r="P38" s="25"/>
@@ -7445,18 +7445,18 @@
         <v>115</v>
       </c>
       <c r="V38" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W38" s="25"/>
       <c r="X38" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y38" s="25" t="s">
         <v>164</v>
-      </c>
-      <c r="Y38" s="25" t="s">
-        <v>165</v>
       </c>
       <c r="Z38" s="25"/>
       <c r="AA38" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AB38" s="25"/>
       <c r="AC38" s="25"/>
@@ -7467,25 +7467,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="G39" t="s">
+        <v>178</v>
+      </c>
+      <c r="H39" t="s">
         <v>385</v>
-      </c>
-      <c r="G39" t="s">
-        <v>179</v>
-      </c>
-      <c r="H39" t="s">
-        <v>386</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7500,16 +7500,16 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>386</v>
+      </c>
+      <c r="X39" t="s">
         <v>387</v>
       </c>
-      <c r="X39" t="s">
-        <v>388</v>
-      </c>
       <c r="Y39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -7542,17 +7542,17 @@
     <hyperlink ref="G9" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
     <hyperlink ref="G16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
     <hyperlink ref="G17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G18" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="G19" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="G32" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G19" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="G32" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G14" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G34" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G2" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G36" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G37" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G38" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G18" r:id="rId36" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
@@ -7561,6 +7561,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7765,41 +7785,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7822,9 +7811,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
M2/M4: integration of group "Fahrzeugart".
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A622B30B-B5E2-42C8-BB06-BFDCFC403D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D715BA9B-418D-4FAA-BEE7-08B59F07AA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-1488" windowWidth="23256" windowHeight="14016" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="401">
   <si>
     <t>#</t>
   </si>
@@ -1045,9 +1045,6 @@
     <t>total_variable=Treibstoffe[alle], share="Anteil Elektrofahrzeuge (ohne Hybrid)": Treibstoff[Elektrisch;Wasserstoff]/Treibstoff[alle]</t>
   </si>
   <si>
-    <t>Antriebsart bei Gütertransportfahrzeugen - Fahrzeugbestand</t>
-  </si>
-  <si>
     <t>Fahrzeugbestand - Antriebsart bei Sachentransportfahrzeugen</t>
   </si>
   <si>
@@ -1060,9 +1057,6 @@
     <t>Benzin,Diesel,Benzin-elektrisch: Normal-Hybrid,Benzin-elektrisch: Plug-in-Hybrid,Diesel-elektrisch: Normal-Hybrid,Elektrisch,Wasserstoff,Gas (mono- und bivalent),Anderer</t>
   </si>
   <si>
-    <t>Anzahl Gütertransportfahrzeuge [Anz.]</t>
-  </si>
-  <si>
     <t>[Antriebsart] -- 1: Benzin, Diesel; 2: "Hybrid" -&gt; [Benzin-elektrisch: Normal-Hybrid,Diesel-elektrisch: Normal-Hybrid]; 3: "PlugIn-Hybrid" -&gt;  [Benzin-elektrisch: Plug-in-Hybrid]; 4: Gas [Gas (mono- und bivalent)], Anderer; 5: Wasserstoff; 6: Elektrisch</t>
   </si>
   <si>
@@ -1087,18 +1081,9 @@
     <t>Neue Inverkehrsetzungen von Strassenfahrzeugen (IVS), Bundesamt für Strassen (ASTRA) - IVZ-Fahrzeuge</t>
   </si>
   <si>
-    <t>Antriebsart bei Gütertransportfahrzeugen - Neuzulassungen</t>
-  </si>
-  <si>
     <t>Neuzulassungen - Antriebsart bei Sachentransportfahrzeugen</t>
   </si>
   <si>
-    <t>Sachentransportfahrzeuge</t>
-  </si>
-  <si>
-    <t>Anzahl Neuzulassungen Gütertransportfahrzeuge [Anz.]</t>
-  </si>
-  <si>
     <t>Durchschnittliche CO₂-Emissionen der Personenwagen</t>
   </si>
   <si>
@@ -1313,6 +1298,30 @@
   </si>
   <si>
     <t>KTZH_00002102_00004163.csv</t>
+  </si>
+  <si>
+    <t>30,35,37,38</t>
+  </si>
+  <si>
+    <t>Lieferwagen,Lastwagen,Sattelmotorfahrzeug,Sattelschlepper</t>
+  </si>
+  <si>
+    <t>Fahrzeugart</t>
+  </si>
+  <si>
+    <t>330,335,337,338</t>
+  </si>
+  <si>
+    <t>Antriebsart bei Sachentransportfahrzeugen - Fahrzeugbestand</t>
+  </si>
+  <si>
+    <t>Antriebsart bei Sachentransportfahrzeugen - Neuzulassungen</t>
+  </si>
+  <si>
+    <t>Anzahl Neuzulassungen Sachentransportfahrzeuge [Anz.]</t>
+  </si>
+  <si>
+    <t>Anzahl Sachentransportfahrzeuge [Anz.]</t>
   </si>
 </sst>
 </file>
@@ -4876,10 +4885,10 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5207,7 +5216,7 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
@@ -5305,10 +5314,10 @@
         <v>190</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5711,7 +5720,7 @@
         <v>232</v>
       </c>
       <c r="U12" s="25" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="V12" s="25" t="s">
         <v>233</v>
@@ -5769,7 +5778,7 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>239</v>
@@ -5795,7 +5804,7 @@
         <v>242</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5918,10 +5927,10 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
@@ -6044,7 +6053,7 @@
         <v>169</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6059,7 +6068,7 @@
         <v>274</v>
       </c>
       <c r="U18" s="25" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="V18" s="25" t="s">
         <v>275</v>
@@ -6431,10 +6440,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>308</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>309</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -6446,7 +6455,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6468,22 +6477,28 @@
         <v>222</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
+      <c r="R24" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="S24" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="T24" s="25" t="s">
+        <v>394</v>
+      </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>313</v>
+        <v>400</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="X24" s="25" t="s">
         <v>228</v>
@@ -6509,10 +6524,10 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
@@ -6546,13 +6561,13 @@
         <v>222</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q25" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="R25" s="25" t="s">
         <v>317</v>
-      </c>
-      <c r="Q25" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>319</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
@@ -6564,13 +6579,13 @@
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="W25" s="35" t="s">
         <v>306</v>
       </c>
       <c r="X25" s="25" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>182</v>
@@ -6593,10 +6608,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>322</v>
+        <v>398</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
@@ -6630,31 +6645,31 @@
         <v>222</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q26" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="R26" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="Q26" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="S26" s="25">
-        <v>300</v>
+      <c r="S26" s="25" t="s">
+        <v>396</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>324</v>
+        <v>394</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>325</v>
+        <v>399</v>
       </c>
       <c r="W26" s="35" t="s">
         <v>306</v>
       </c>
       <c r="X26" s="25" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>182</v>
@@ -6677,22 +6692,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H27" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6702,14 +6717,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>161</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6717,29 +6732,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>164</v>
       </c>
       <c r="Z27" s="25" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="AA27" s="25" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6750,32 +6765,32 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
@@ -6784,7 +6799,7 @@
         <v>180</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6812,7 +6827,7 @@
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6823,7 +6838,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6855,7 +6870,7 @@
         <v>180</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6866,7 +6881,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6875,7 +6890,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6890,10 +6905,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6935,7 +6950,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6961,10 +6976,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
@@ -6976,7 +6991,7 @@
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6989,31 +7004,31 @@
         <v>189</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>161</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="V31" s="25" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="X31" s="25" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>164</v>
@@ -7027,25 +7042,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H32" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7055,7 +7070,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7071,7 +7086,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>164</v>
@@ -7090,10 +7105,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7105,7 +7120,7 @@
         <v>178</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7117,7 +7132,7 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
@@ -7126,7 +7141,7 @@
         <v>293</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>164</v>
@@ -7140,35 +7155,35 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
@@ -7177,7 +7192,7 @@
         <v>180</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7229,7 +7244,7 @@
         <v>178</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7246,11 +7261,11 @@
         <v>180</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7259,11 +7274,11 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="Y35" s="25" t="s">
         <v>220</v>
@@ -7300,7 +7315,7 @@
         <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7312,7 +7327,7 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
@@ -7335,13 +7350,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>156</v>
@@ -7356,7 +7371,7 @@
         <v>159</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7401,13 +7416,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>156</v>
@@ -7422,7 +7437,7 @@
         <v>159</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7467,25 +7482,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>383</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>389</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>388</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G39" t="s">
         <v>178</v>
       </c>
       <c r="H39" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7500,10 +7515,10 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="X39" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="Y39" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
M2/M4: some minor adaptions
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D715BA9B-418D-4FAA-BEE7-08B59F07AA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81C7F56-C487-40EC-8D03-0B04F690B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="396">
   <si>
     <t>#</t>
   </si>
@@ -697,9 +697,6 @@
     <t>Gebäude (Anzahl)</t>
   </si>
   <si>
-    <t>Gebäude</t>
-  </si>
-  <si>
     <t>1: Heizöl;2: Gas;3: Elektrizität;4: Holz: [Holz (generisch),Holz (Pellets),Holz (Schnitzel),Holz (Stückholz)];5: Sonne: [Sonne (thermisch)];6: Wärmepumpe: [Wärmepumpe (Wasser),Wärmepumpe (Luft),Wärmepumpe (Gas),Wärmepumpe (Fernwärme),Wärmepumpe (Erdwärme),Wärmepumpe (Erdwärmesonde),Wärmepumpe (Erdregister),Wärmepumpe (andere Quelle),Wärmepumpe (unbestimmte Quelle)];7: Fernwärme: [Fernwärme (generisch),Fernwärme (Hochtemperatur),Fernwärme (Niedertemperatur)];8: Andere: [Abwärme (innerhalb des Gebäudes), Andere, Keine, Unbestimmt]</t>
   </si>
   <si>
@@ -799,9 +796,6 @@
     <t>Industriefahrzeuge (Anzahl)</t>
   </si>
   <si>
-    <t>Industriefahrzeuge</t>
-  </si>
-  <si>
     <t>[Antriebsart] -- 1: Benzin, Diesel; 2: "Hybrid" -&gt; [Benzin-elektrisch: Hybrid,Diesel-elektrisch: Hybrid]; 3: Gas [Gas (mono- und bivalent)], Anderer; 4: Wasserstoff; 5: Elektrisch</t>
   </si>
   <si>
@@ -886,9 +880,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>Vertankte Menge Sustainable Aviation Fuel (SAF)</t>
-  </si>
-  <si>
     <t>Bundesamt für Zivilluftfahrt (BAZL)</t>
   </si>
   <si>
@@ -907,9 +898,6 @@
     <t>kg CO₂/m²</t>
   </si>
   <si>
-    <t>CO₂-Emissionen in kg pro m²</t>
-  </si>
-  <si>
     <t>Hochbauamt des Kantons Zürich</t>
   </si>
   <si>
@@ -958,9 +946,6 @@
     <t>Antriebstechnologie: Benzin,Diesel,Hybid,PlugIn-Hybrid,Gas,Elektro,Wasserstoff,Andere</t>
   </si>
   <si>
-    <t>Fahrzeuge [Anz.], differenziert nach Fahrzeugstyp und Antriebstechnologien</t>
-  </si>
-  <si>
     <t>[Antriebstechnologie] -- 1: Benzin, Diesel; 2: Hybrid; 3: PlugIn-Hybrid; 4: Gas, Andere; 5: Wasserstoff; 6: Elektro</t>
   </si>
   <si>
@@ -1012,9 +997,6 @@
     <t>Benzin,Diesel,Benzin-elektrisch: Hybrid,Diesel-elektrisch: Hybrid,Elektrisch,Gas (mono- und bivalent),Anderer</t>
   </si>
   <si>
-    <t>Landwirtschaftsfahrzeuge [Anz.]</t>
-  </si>
-  <si>
     <t>[Antriebsart] -- 1: Benzin, Diesel; 2: "Hybrid" -&gt; [Benzin-elektrisch: Hybrid,Diesel-elektrisch: Hybrid]; 3: Gas [Gas (mono- und bivalent)], Anderer; 4: Elektrisch</t>
   </si>
   <si>
@@ -1033,9 +1015,6 @@
     <t>Benzin,Diesel,Benzin-elektrisch: Normal-Hybrid,Benzin-elektrisch: Plug-in-Hybrid,Diesel-elektrisch: Normal-Hybrid,Diesel-elektrisch: Plug-in-Hybrid,Elektrisch,Wasserstoff,Gas (mono- und bivalent),Anderer</t>
   </si>
   <si>
-    <t>Bestand der Personenwagen</t>
-  </si>
-  <si>
     <t>Personenwagen</t>
   </si>
   <si>
@@ -1075,9 +1054,6 @@
     <t>Fahrzeuggruppe / -art</t>
   </si>
   <si>
-    <t>Anzahl Neuzulassungen PW [Anz.]</t>
-  </si>
-  <si>
     <t>Neue Inverkehrsetzungen von Strassenfahrzeugen (IVS), Bundesamt für Strassen (ASTRA) - IVZ-Fahrzeuge</t>
   </si>
   <si>
@@ -1318,10 +1294,19 @@
     <t>Antriebsart bei Sachentransportfahrzeugen - Neuzulassungen</t>
   </si>
   <si>
-    <t>Anzahl Neuzulassungen Sachentransportfahrzeuge [Anz.]</t>
-  </si>
-  <si>
-    <t>Anzahl Sachentransportfahrzeuge [Anz.]</t>
+    <t>Tonnen Stickstoffdünger</t>
+  </si>
+  <si>
+    <t>Fahrzeuge [Anz.]</t>
+  </si>
+  <si>
+    <t>SAF [t/a]</t>
+  </si>
+  <si>
+    <t>Gebäude [Anz.]</t>
+  </si>
+  <si>
+    <t>CO₂-Emissionen [kg/m²]</t>
   </si>
 </sst>
 </file>
@@ -4885,10 +4870,10 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5216,7 +5201,7 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
@@ -5314,10 +5299,10 @@
         <v>190</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5326,19 +5311,19 @@
         <v>191</v>
       </c>
       <c r="V6" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="W6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="W6" s="25" t="s">
+      <c r="X6" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="X6" s="25" t="s">
-        <v>194</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z6" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>184</v>
@@ -5358,7 +5343,7 @@
         <v>89</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>91</v>
@@ -5370,7 +5355,7 @@
         <v>178</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>86</v>
@@ -5384,7 +5369,7 @@
         <v>180</v>
       </c>
       <c r="O7" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q7" s="25" t="s">
         <v>181</v>
@@ -5406,7 +5391,7 @@
         <v>164</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>184</v>
@@ -5423,7 +5408,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
@@ -5435,10 +5420,10 @@
         <v>178</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>201</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>202</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
@@ -5448,31 +5433,31 @@
         <v>180</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>204</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>205</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5486,19 +5471,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>210</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>211</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5514,7 +5499,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5527,14 +5512,14 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>164</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
@@ -5548,10 +5533,10 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>214</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>215</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
@@ -5563,7 +5548,7 @@
         <v>178</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5577,31 +5562,31 @@
         <v>180</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
@@ -5618,7 +5603,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
@@ -5648,31 +5633,31 @@
         <v>161</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="W11" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="V11" s="25" t="s">
+      <c r="X11" s="25" t="s">
         <v>226</v>
-      </c>
-      <c r="W11" s="35" t="s">
-        <v>227</v>
-      </c>
-      <c r="X11" s="25" t="s">
-        <v>228</v>
       </c>
       <c r="Y11" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z11" s="25" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>184</v>
@@ -5689,7 +5674,7 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
@@ -5701,7 +5686,7 @@
         <v>178</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5713,17 +5698,17 @@
         <v>180</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="U12" s="25" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5734,7 +5719,7 @@
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -5748,10 +5733,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
@@ -5760,13 +5745,13 @@
         <v>187</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="I13" s="25" t="s">
         <v>236</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>238</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5778,19 +5763,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="V13" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="X13" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5801,10 +5786,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5816,7 +5801,7 @@
         <v>178</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5826,28 +5811,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>161</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="U14" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="V14" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>164</v>
@@ -5867,19 +5852,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>178</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5891,26 +5876,26 @@
         <v>189</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q15" s="25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="U15" s="25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="V15" s="25" t="s">
-        <v>255</v>
+        <v>393</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>164</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>184</v>
@@ -5927,22 +5912,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>178</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5951,23 +5936,23 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="U16" s="25" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>262</v>
+        <v>395</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -5984,19 +5969,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>178</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -6005,26 +5990,26 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Q17" s="25" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="U17" s="25" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>176</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Y17" s="25" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AA17" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -6038,10 +6023,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
@@ -6053,7 +6038,7 @@
         <v>169</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6062,20 +6047,20 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="Q18" s="25" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="U18" s="25" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="V18" s="25" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="Y18" s="25" t="s">
         <v>182</v>
@@ -6096,10 +6081,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
@@ -6123,31 +6108,31 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>279</v>
+        <v>392</v>
       </c>
       <c r="W19" s="35" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="X19" s="25" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="Y19" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>184</v>
@@ -6164,7 +6149,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
@@ -6176,7 +6161,7 @@
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6185,7 +6170,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6194,13 +6179,13 @@
         <v>161</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6209,16 +6194,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="X20" s="25" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6232,7 +6217,7 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
@@ -6244,7 +6229,7 @@
         <v>178</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6256,14 +6241,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6274,7 +6259,7 @@
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
@@ -6291,7 +6276,7 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
@@ -6321,13 +6306,13 @@
         <v>161</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P22" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="Q22" s="25" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6336,19 +6321,19 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>297</v>
+        <v>392</v>
       </c>
       <c r="W22" s="35" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="X22" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Y22" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AA22" s="25" t="s">
         <v>184</v>
@@ -6362,10 +6347,10 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
@@ -6396,34 +6381,34 @@
         <v>161</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="Q23" s="25" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25" t="s">
-        <v>304</v>
+        <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>305</v>
+        <v>392</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="X23" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Y23" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AA23" s="25" t="s">
         <v>184</v>
@@ -6440,10 +6425,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -6455,7 +6440,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6474,40 +6459,40 @@
         <v>161</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="Q24" s="25" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="X24" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Y24" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AA24" s="25" t="s">
         <v>184</v>
@@ -6524,10 +6509,10 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
@@ -6558,40 +6543,40 @@
         <v>161</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="Q25" s="25" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>318</v>
+        <v>392</v>
       </c>
       <c r="W25" s="35" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="X25" s="25" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AA25" s="25" t="s">
         <v>184</v>
@@ -6608,10 +6593,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
@@ -6642,40 +6627,40 @@
         <v>161</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="Q26" s="25" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="R26" s="25" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="W26" s="35" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="X26" s="25" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>182</v>
       </c>
       <c r="Z26" s="25" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>184</v>
@@ -6692,22 +6677,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H27" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6717,14 +6702,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>161</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6732,29 +6717,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>164</v>
       </c>
       <c r="Z27" s="25" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="AA27" s="25" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6765,32 +6750,32 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
@@ -6799,7 +6784,7 @@
         <v>180</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6810,24 +6795,24 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6838,7 +6823,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6870,7 +6855,7 @@
         <v>180</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6881,7 +6866,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6890,7 +6875,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6905,10 +6890,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6938,10 +6923,10 @@
         <v>171</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6950,7 +6935,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6976,10 +6961,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
@@ -6991,7 +6976,7 @@
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -7004,37 +6989,37 @@
         <v>189</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>161</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="V31" s="25" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="X31" s="25" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -7042,25 +7027,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H32" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7070,7 +7055,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7086,7 +7071,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>164</v>
@@ -7105,10 +7090,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7120,7 +7105,7 @@
         <v>178</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7132,22 +7117,22 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -7155,35 +7140,35 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
@@ -7192,7 +7177,7 @@
         <v>180</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7203,18 +7188,18 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
@@ -7244,7 +7229,7 @@
         <v>178</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7261,11 +7246,11 @@
         <v>180</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7274,18 +7259,18 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
@@ -7315,7 +7300,7 @@
         <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7327,22 +7312,22 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>164</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -7350,13 +7335,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>156</v>
@@ -7371,7 +7356,7 @@
         <v>159</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7416,13 +7401,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>154</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>156</v>
@@ -7437,7 +7422,7 @@
         <v>159</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7482,25 +7467,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G39" t="s">
         <v>178</v>
       </c>
       <c r="H39" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7515,16 +7500,16 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="X39" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="Y39" t="s">
         <v>164</v>
       </c>
       <c r="AA39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -7576,26 +7561,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7800,10 +7765,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7826,20 +7822,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Hotfix for issue #31 - LF1: change in time series
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corinna.grobe@zh.ch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81C7F56-C487-40EC-8D03-0B04F690B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5474AC4-544E-4D02-9826-E1482C9A7E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -81,7 +81,11 @@
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
-    Jährliche Daten erst seit 1996 verfügbar, deshalb dort Start auch wenn erste Daten aus 1975 stammen.</t>
+    Jährliche Daten erst seit 1996 verfügbar, deshalb dort Start auch wenn erste Daten aus 1975 stammen.
+Antwort:
+    In einigen Fällen wird das Jahr nicht durch den Wert der Jahreszahl angegeben, z. B. „2023“, sondern durch einen Index, wobei das jüngste Jahr „0“ ist. 
+LF1 ist so ein Fall.
+Es wird die Anzahl Jahre abgefragt, also 2023-1996 = 27</t>
       </text>
     </comment>
     <comment ref="H31" authorId="2" shapeId="0" xr:uid="{AE0623BC-6FA4-49C9-B450-941BCEB6A906}">
@@ -2423,6 +2427,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Gian-Marco Alt" id="{9E374A6E-78EE-4895-9219-03BB83C00527}" userId="Gian-Marco Alt" providerId="None"/>
+  <person displayName="Corinna" id="{8ACF132E-3FF5-4FD0-A246-4EA4B6356232}" userId="S::corinna.grobe@zh.ch::28e595fc-7a83-47b8-a91d-60e5cb3ed20d" providerId="AD"/>
   <person displayName="Gastbenutzer" id="{808E65DB-4307-4BA3-BC76-03CCDC34E544}" userId="S::urn:spo:anon#04ba5703d9ed7f2f793f586646c8093f7ea625b86d77f95d6c68abd8d0af7a17::" providerId="AD"/>
 </personList>
 </file>
@@ -2700,6 +2705,11 @@
   <threadedComment ref="K20" dT="2023-05-03T08:29:37.28" personId="{808E65DB-4307-4BA3-BC76-03CCDC34E544}" id="{F8D71A7C-E5F7-4AB2-BA3A-263385823BB9}">
     <text>Jährliche Daten erst seit 1996 verfügbar, deshalb dort Start auch wenn erste Daten aus 1975 stammen.</text>
   </threadedComment>
+  <threadedComment ref="K20" dT="2024-05-16T09:56:34.54" personId="{8ACF132E-3FF5-4FD0-A246-4EA4B6356232}" id="{FB937496-4D68-4F54-9C2D-D2C2622786E8}" parentId="{F8D71A7C-E5F7-4AB2-BA3A-263385823BB9}">
+    <text>In einigen Fällen wird das Jahr nicht durch den Wert der Jahreszahl angegeben, z. B. „2023“, sondern durch einen Index, wobei das jüngste Jahr „0“ ist. 
+LF1 ist so ein Fall.
+Es wird die Anzahl Jahre abgefragt, also 2023-1996 = 27</text>
+  </threadedComment>
   <threadedComment ref="H31" dT="2024-01-10T12:59:42.39" personId="{9E374A6E-78EE-4895-9219-03BB83C00527}" id="{AE0623BC-6FA4-49C9-B450-941BCEB6A906}">
     <text>px-x-0103010000_102 ersetzt durch px-x-0102020000_101</text>
   </threadedComment>
@@ -2721,24 +2731,24 @@
       <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.125" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.1640625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.1640625" style="2"/>
-    <col min="6" max="6" width="16.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.1640625" style="2"/>
-    <col min="13" max="13" width="15.1640625" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.1640625" style="2"/>
-    <col min="16" max="17" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.1640625" style="2"/>
+    <col min="1" max="1" width="6.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.125" style="2"/>
+    <col min="6" max="6" width="16.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="2" customWidth="1"/>
+    <col min="10" max="12" width="10.125" style="2"/>
+    <col min="13" max="13" width="15.125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.125" style="2"/>
+    <col min="16" max="17" width="17.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.125" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:11" ht="104.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="103.8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -4870,43 +4880,43 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V7" sqref="V7"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.5" customWidth="1"/>
-    <col min="4" max="4" width="111.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="138.1640625" customWidth="1"/>
-    <col min="8" max="8" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="138.125" customWidth="1"/>
+    <col min="8" max="8" width="49.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="49.5" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="69" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="160.5" customWidth="1"/>
     <col min="21" max="21" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="93.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="93.1640625" customWidth="1"/>
+    <col min="22" max="22" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="93.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="93.125" customWidth="1"/>
     <col min="26" max="26" width="25.5" customWidth="1"/>
-    <col min="27" max="27" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>123</v>
       </c>
@@ -5001,7 +5011,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -5070,7 +5080,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -5130,7 +5140,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>1</v>
       </c>
@@ -5190,7 +5200,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>1</v>
       </c>
@@ -5254,7 +5264,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>1</v>
       </c>
@@ -5332,7 +5342,7 @@
       <c r="AC6" s="25"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>1</v>
       </c>
@@ -5397,7 +5407,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>1</v>
       </c>
@@ -5460,7 +5470,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>1</v>
       </c>
@@ -5525,7 +5535,7 @@
       <c r="AC9" s="25"/>
       <c r="AD9" s="25"/>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>1</v>
       </c>
@@ -5592,7 +5602,7 @@
       <c r="AC10" s="25"/>
       <c r="AD10" s="25"/>
     </row>
-    <row r="11" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>1</v>
       </c>
@@ -5663,7 +5673,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -5725,7 +5735,7 @@
       <c r="AC12"/>
       <c r="AD12"/>
     </row>
-    <row r="13" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>1</v>
       </c>
@@ -5778,7 +5788,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>1</v>
       </c>
@@ -5841,7 +5851,7 @@
       <c r="AC14"/>
       <c r="AD14"/>
     </row>
-    <row r="15" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>1</v>
       </c>
@@ -5904,7 +5914,7 @@
       <c r="AC15"/>
       <c r="AD15"/>
     </row>
-    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>1</v>
       </c>
@@ -5958,7 +5968,7 @@
       <c r="AC16"/>
       <c r="AD16"/>
     </row>
-    <row r="17" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>1</v>
       </c>
@@ -6015,7 +6025,7 @@
       <c r="AC17"/>
       <c r="AD17"/>
     </row>
-    <row r="18" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>1</v>
       </c>
@@ -6073,7 +6083,7 @@
       <c r="AC18"/>
       <c r="AD18"/>
     </row>
-    <row r="19" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>1</v>
       </c>
@@ -6138,7 +6148,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>1</v>
       </c>
@@ -6167,7 +6177,8 @@
         <v>86</v>
       </c>
       <c r="K20" s="25">
-        <v>1996</v>
+        <f>2023-1996</f>
+        <v>27</v>
       </c>
       <c r="L20" t="s">
         <v>279</v>
@@ -6206,7 +6217,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>1</v>
       </c>
@@ -6265,7 +6276,7 @@
       <c r="AC21" s="25"/>
       <c r="AD21" s="25"/>
     </row>
-    <row r="22" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>1</v>
       </c>
@@ -6339,7 +6350,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>1</v>
       </c>
@@ -6417,7 +6428,7 @@
       <c r="AC23" s="25"/>
       <c r="AD23" s="25"/>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>1</v>
       </c>
@@ -6501,7 +6512,7 @@
       <c r="AC24" s="25"/>
       <c r="AD24" s="25"/>
     </row>
-    <row r="25" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>1</v>
       </c>
@@ -6585,7 +6596,7 @@
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
     </row>
-    <row r="26" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>1</v>
       </c>
@@ -6669,7 +6680,7 @@
       <c r="AC26" s="25"/>
       <c r="AD26" s="25"/>
     </row>
-    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>1</v>
       </c>
@@ -6742,7 +6753,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>1</v>
       </c>
@@ -6815,7 +6826,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>0</v>
       </c>
@@ -6882,7 +6893,7 @@
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
     </row>
-    <row r="30" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>1</v>
       </c>
@@ -6953,7 +6964,7 @@
       <c r="AD30" s="25"/>
       <c r="AE30" s="25"/>
     </row>
-    <row r="31" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>1</v>
       </c>
@@ -7022,7 +7033,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>1</v>
       </c>
@@ -7082,7 +7093,7 @@
       <c r="AC32" s="25"/>
       <c r="AD32" s="25"/>
     </row>
-    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>1</v>
       </c>
@@ -7135,7 +7146,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>1</v>
       </c>
@@ -7206,7 +7217,7 @@
       <c r="AD34" s="25"/>
       <c r="AE34" s="25"/>
     </row>
-    <row r="35" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>1</v>
       </c>
@@ -7277,7 +7288,7 @@
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
     </row>
-    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25">
         <v>1</v>
       </c>
@@ -7330,7 +7341,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>1</v>
       </c>
@@ -7396,7 +7407,7 @@
       <c r="AC37" s="25"/>
       <c r="AD37" s="25"/>
     </row>
-    <row r="38" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>1</v>
       </c>
@@ -7462,7 +7473,7 @@
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
     </row>
-    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>1</v>
       </c>
@@ -7561,6 +7572,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7765,17 +7787,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7786,6 +7797,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7804,27 +7832,16 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ab6d1c10-a186-47ab-af91-cdbff51004f3}" enabled="1" method="Standard" siteId="{a020d0ae-094a-4d44-b66c-ac3fe8e90c58}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
fix: new Excel list with year_start logic implemented
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corinna.grobe@zh.ch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp.bosch@zh.ch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5474AC4-544E-4D02-9826-E1482C9A7E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E651E-A2F5-460D-AD07-C27046586ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2731,24 +2731,24 @@
       <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.125" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.125" style="2"/>
-    <col min="6" max="6" width="16.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.125" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.125" style="2"/>
-    <col min="13" max="13" width="15.125" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.125" style="2"/>
-    <col min="16" max="17" width="17.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.125" style="2"/>
+    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.109375" style="2"/>
+    <col min="6" max="6" width="16.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="10.109375" style="2"/>
+    <col min="13" max="13" width="15.109375" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.109375" style="2"/>
+    <col min="16" max="17" width="17.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:11" ht="103.8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.01</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1.02</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>1.03</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1.04</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>23</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>25</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>33</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>34</v>
       </c>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>35</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>36</v>
       </c>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>37</v>
       </c>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>38</v>
       </c>
@@ -4228,7 +4228,7 @@
       </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>39</v>
       </c>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>40</v>
       </c>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>41</v>
       </c>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>42</v>
       </c>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>43</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>45</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>47</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>48</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>49</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>50</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>51</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <f>SUBTOTAL(103,Über112['#])</f>
         <v>45</v>
@@ -4880,43 +4880,43 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.5" customWidth="1"/>
-    <col min="4" max="4" width="111.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="138.125" customWidth="1"/>
-    <col min="8" max="8" width="49.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.5" customWidth="1"/>
-    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.44140625" customWidth="1"/>
+    <col min="4" max="4" width="111.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="138.109375" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="69" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="160.5" customWidth="1"/>
-    <col min="21" max="21" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="93.125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="93.125" customWidth="1"/>
-    <col min="26" max="26" width="25.5" customWidth="1"/>
-    <col min="27" max="27" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="160.44140625" customWidth="1"/>
+    <col min="21" max="21" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="93.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="93.109375" customWidth="1"/>
+    <col min="26" max="26" width="25.44140625" customWidth="1"/>
+    <col min="27" max="27" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>123</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>1</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <v>1</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <v>1</v>
       </c>
@@ -5342,7 +5342,7 @@
       <c r="AC6" s="25"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <v>1</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <v>1</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
         <v>1</v>
       </c>
@@ -5535,7 +5535,7 @@
       <c r="AC9" s="25"/>
       <c r="AD9" s="25"/>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
         <v>1</v>
       </c>
@@ -5602,7 +5602,7 @@
       <c r="AC10" s="25"/>
       <c r="AD10" s="25"/>
     </row>
-    <row r="11" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <v>1</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -5735,7 +5735,7 @@
       <c r="AC12"/>
       <c r="AD12"/>
     </row>
-    <row r="13" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <v>1</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <v>1</v>
       </c>
@@ -5851,7 +5851,7 @@
       <c r="AC14"/>
       <c r="AD14"/>
     </row>
-    <row r="15" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <v>1</v>
       </c>
@@ -5914,7 +5914,7 @@
       <c r="AC15"/>
       <c r="AD15"/>
     </row>
-    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <v>1</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="AC16"/>
       <c r="AD16"/>
     </row>
-    <row r="17" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
         <v>1</v>
       </c>
@@ -6025,7 +6025,7 @@
       <c r="AC17"/>
       <c r="AD17"/>
     </row>
-    <row r="18" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <v>1</v>
       </c>
@@ -6083,7 +6083,7 @@
       <c r="AC18"/>
       <c r="AD18"/>
     </row>
-    <row r="19" spans="1:31" s="25" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <v>1</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <v>1</v>
       </c>
@@ -6177,8 +6177,7 @@
         <v>86</v>
       </c>
       <c r="K20" s="25">
-        <f>2023-1996</f>
-        <v>27</v>
+        <v>1996</v>
       </c>
       <c r="L20" t="s">
         <v>279</v>
@@ -6217,7 +6216,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>1</v>
       </c>
@@ -6276,7 +6275,7 @@
       <c r="AC21" s="25"/>
       <c r="AD21" s="25"/>
     </row>
-    <row r="22" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>1</v>
       </c>
@@ -6350,7 +6349,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
         <v>1</v>
       </c>
@@ -6428,7 +6427,7 @@
       <c r="AC23" s="25"/>
       <c r="AD23" s="25"/>
     </row>
-    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="25">
         <v>1</v>
       </c>
@@ -6512,7 +6511,7 @@
       <c r="AC24" s="25"/>
       <c r="AD24" s="25"/>
     </row>
-    <row r="25" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A25" s="25">
         <v>1</v>
       </c>
@@ -6596,7 +6595,7 @@
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
     </row>
-    <row r="26" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <v>1</v>
       </c>
@@ -6680,7 +6679,7 @@
       <c r="AC26" s="25"/>
       <c r="AD26" s="25"/>
     </row>
-    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="25">
         <v>1</v>
       </c>
@@ -6753,7 +6752,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="28" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
         <v>1</v>
       </c>
@@ -6826,7 +6825,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="29" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <v>0</v>
       </c>
@@ -6893,7 +6892,7 @@
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
     </row>
-    <row r="30" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <v>1</v>
       </c>
@@ -6964,7 +6963,7 @@
       <c r="AD30" s="25"/>
       <c r="AE30" s="25"/>
     </row>
-    <row r="31" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <v>1</v>
       </c>
@@ -7033,7 +7032,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="25">
         <v>1</v>
       </c>
@@ -7093,7 +7092,7 @@
       <c r="AC32" s="25"/>
       <c r="AD32" s="25"/>
     </row>
-    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <v>1</v>
       </c>
@@ -7146,7 +7145,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="25">
         <v>1</v>
       </c>
@@ -7217,7 +7216,7 @@
       <c r="AD34" s="25"/>
       <c r="AE34" s="25"/>
     </row>
-    <row r="35" spans="1:31" s="28" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A35" s="25">
         <v>1</v>
       </c>
@@ -7288,7 +7287,7 @@
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
     </row>
-    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25">
         <v>1</v>
       </c>
@@ -7341,7 +7340,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>1</v>
       </c>
@@ -7407,7 +7406,7 @@
       <c r="AC37" s="25"/>
       <c r="AD37" s="25"/>
     </row>
-    <row r="38" spans="1:31" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
         <v>1</v>
       </c>
@@ -7473,7 +7472,7 @@
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
     </row>
-    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25">
         <v>1</v>
       </c>
@@ -7583,6 +7582,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7787,15 +7795,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
@@ -7814,6 +7813,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7832,14 +7839,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{ab6d1c10-a186-47ab-af91-cdbff51004f3}" enabled="1" method="Standard" siteId="{a020d0ae-094a-4d44-b66c-ac3fe8e90c58}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
KV4: Anpassung URL -> OGD
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp.bosch@zh.ch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2E651E-A2F5-460D-AD07-C27046586ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD33483-8178-4E51-9937-92805AD02D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -491,9 +491,6 @@
     <t>Stromerzeugung mit Photovoltaik auf kantonalen Gebäuden</t>
   </si>
   <si>
-    <t>KV4_data.csv</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -1311,6 +1308,9 @@
   </si>
   <si>
     <t>CO₂-Emissionen [kg/m²]</t>
+  </si>
+  <si>
+    <t>KTZH_00002102_00004164.csv</t>
   </si>
 </sst>
 </file>
@@ -2731,24 +2731,24 @@
       <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.109375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.109375" style="2"/>
-    <col min="6" max="6" width="16.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.109375" style="2"/>
-    <col min="13" max="13" width="15.109375" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.109375" style="2"/>
-    <col min="16" max="17" width="17.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.109375" style="2"/>
+    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.1640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.1640625" style="2"/>
+    <col min="6" max="6" width="16.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
+    <col min="10" max="12" width="10.1640625" style="2"/>
+    <col min="13" max="13" width="15.1640625" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.1640625" style="2"/>
+    <col min="16" max="17" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:11" ht="103.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:11" ht="104.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>1.01</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>1.02</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>1.03</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>1.04</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>23</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>25</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>33</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>34</v>
       </c>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>35</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>36</v>
       </c>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>37</v>
       </c>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>38</v>
       </c>
@@ -4228,7 +4228,7 @@
       </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>39</v>
       </c>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>40</v>
       </c>
@@ -4320,7 +4320,7 @@
       </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>41</v>
       </c>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>42</v>
       </c>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>43</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>45</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>47</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>48</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>49</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>50</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>51</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
         <f>SUBTOTAL(103,Über112['#])</f>
         <v>45</v>
@@ -4880,138 +4880,138 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.44140625" customWidth="1"/>
-    <col min="4" max="4" width="111.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="138.109375" customWidth="1"/>
-    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.5" customWidth="1"/>
+    <col min="4" max="4" width="111.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="138.1640625" customWidth="1"/>
+    <col min="8" max="8" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.5" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="69" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="160.44140625" customWidth="1"/>
-    <col min="21" max="21" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="93.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="93.109375" customWidth="1"/>
-    <col min="26" max="26" width="25.44140625" customWidth="1"/>
-    <col min="27" max="27" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="160.5" customWidth="1"/>
+    <col min="21" max="21" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="93.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="93.1640625" customWidth="1"/>
+    <col min="26" max="26" width="25.5" customWidth="1"/>
+    <col min="27" max="27" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="K1" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="L1" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="X1" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="Y1" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Z1" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AA1" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AB1" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AC1" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AE1" t="s">
         <v>152</v>
       </c>
-      <c r="AE1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -5019,25 +5019,25 @@
         <v>68</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="H2" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>159</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>160</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>86</v>
@@ -5048,7 +5048,7 @@
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O2" s="25"/>
       <c r="P2" s="25"/>
@@ -5060,27 +5060,27 @@
         <v>108</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W2" s="25"/>
       <c r="X2" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y2" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="Y2" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="Z2" s="25"/>
       <c r="AA2" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB2" s="25"/>
       <c r="AC2" s="25"/>
       <c r="AD2" s="25"/>
       <c r="AE2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -5091,19 +5091,19 @@
         <v>114</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="25" t="s">
         <v>169</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>170</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>86</v>
@@ -5115,11 +5115,11 @@
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P3" s="25"/>
       <c r="Q3" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R3" s="25"/>
       <c r="S3" s="25"/>
@@ -5128,19 +5128,19 @@
         <v>115</v>
       </c>
       <c r="V3" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X3" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y3" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA3" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="25">
         <v>1</v>
       </c>
@@ -5151,19 +5151,19 @@
         <v>116</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F4" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>169</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>170</v>
       </c>
       <c r="J4" s="25" t="s">
         <v>86</v>
@@ -5175,11 +5175,11 @@
       <c r="M4" s="25"/>
       <c r="N4" s="25"/>
       <c r="O4" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P4" s="25"/>
       <c r="Q4" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R4" s="25"/>
       <c r="S4" s="25"/>
@@ -5188,19 +5188,19 @@
         <v>115</v>
       </c>
       <c r="V4" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X4" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y4" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA4" s="25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
         <v>1</v>
       </c>
@@ -5211,19 +5211,19 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="H5" s="25" t="s">
         <v>178</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>179</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>86</v>
@@ -5233,13 +5233,13 @@
       </c>
       <c r="L5" s="25"/>
       <c r="N5" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q5" s="25" t="s">
         <v>180</v>
-      </c>
-      <c r="O5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>181</v>
       </c>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
@@ -5248,23 +5248,23 @@
         <v>115</v>
       </c>
       <c r="V5" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W5" s="25"/>
       <c r="X5" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y5" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z5" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="AA5" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
         <v>1</v>
       </c>
@@ -5272,22 +5272,22 @@
         <v>53</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>186</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25" t="s">
@@ -5297,52 +5297,52 @@
         <v>2021</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M6" s="25">
         <v>0.1</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P6" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q6" s="25" t="s">
         <v>378</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>379</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="W6" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="V6" s="25" t="s">
-        <v>394</v>
-      </c>
-      <c r="W6" s="25" t="s">
+      <c r="X6" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="Y6" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z6" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="Y6" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z6" s="32" t="s">
-        <v>194</v>
-      </c>
       <c r="AA6" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="25">
         <v>1</v>
       </c>
@@ -5353,19 +5353,19 @@
         <v>89</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H7" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>86</v>
@@ -5376,13 +5376,13 @@
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
       <c r="N7" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>180</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>181</v>
       </c>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
@@ -5391,23 +5391,23 @@
         <v>115</v>
       </c>
       <c r="V7" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W7" s="25"/>
       <c r="X7" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y7" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25">
         <v>1</v>
       </c>
@@ -5418,59 +5418,59 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>200</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>201</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
       </c>
       <c r="L8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>203</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>204</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="25">
         <v>1</v>
       </c>
@@ -5481,19 +5481,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>209</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>210</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5504,12 +5504,12 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5522,20 +5522,20 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y9" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
       <c r="AD9" s="25"/>
     </row>
-    <row r="10" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>1</v>
       </c>
@@ -5543,22 +5543,22 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>213</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>214</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F10" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H10" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5569,40 +5569,40 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
       <c r="AD10" s="25"/>
     </row>
-    <row r="11" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
         <v>1</v>
       </c>
@@ -5613,13 +5613,13 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>104</v>
@@ -5634,46 +5634,46 @@
         <v>2005</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M11" s="25">
         <v>0.1</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="W11" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="V11" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="W11" s="35" t="s">
+      <c r="X11" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="X11" s="25" t="s">
+      <c r="Y11" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z11" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="Y11" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>227</v>
-      </c>
       <c r="AA11" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -5684,19 +5684,19 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5705,37 +5705,37 @@
         <v>2020</v>
       </c>
       <c r="N12" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="U12" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>230</v>
-      </c>
-      <c r="U12" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>231</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y12" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
       <c r="AD12"/>
     </row>
-    <row r="13" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="25">
         <v>1</v>
       </c>
@@ -5743,25 +5743,25 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>232</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>233</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>235</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>236</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5773,22 +5773,22 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="X13" s="25" t="s">
+      <c r="Y13" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA13" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="Y13" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="AA13" s="25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="25">
         <v>1</v>
       </c>
@@ -5796,22 +5796,22 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H14" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5821,37 +5821,37 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>246</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y14" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB14"/>
       <c r="AC14"/>
       <c r="AD14"/>
     </row>
-    <row r="15" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="25">
         <v>1</v>
       </c>
@@ -5862,19 +5862,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" s="25" t="s">
         <v>249</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>250</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5883,38 +5883,38 @@
         <v>2021</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="U15" s="25" t="s">
-        <v>252</v>
-      </c>
       <c r="V15" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y15" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z15" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="Y15" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z15" s="25" t="s">
-        <v>254</v>
-      </c>
       <c r="AA15" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB15"/>
       <c r="AC15"/>
       <c r="AD15"/>
     </row>
-    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
         <v>1</v>
       </c>
@@ -5922,22 +5922,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>366</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>367</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" s="25" t="s">
         <v>255</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>256</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5946,29 +5946,29 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="U16" s="25" t="s">
-        <v>258</v>
-      </c>
       <c r="V16" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y16" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
       <c r="AD16"/>
     </row>
-    <row r="17" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>1</v>
       </c>
@@ -5979,19 +5979,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -6000,32 +6000,32 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="U17" s="25" t="s">
-        <v>264</v>
-      </c>
       <c r="V17" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="Y17" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="AA17" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
       <c r="AD17"/>
     </row>
-    <row r="18" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>1</v>
       </c>
@@ -6033,22 +6033,22 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>267</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>268</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F18" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>169</v>
-      </c>
       <c r="H18" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6057,33 +6057,33 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>270</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>271</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y18" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z18"/>
       <c r="AA18" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB18"/>
       <c r="AC18"/>
       <c r="AD18"/>
     </row>
-    <row r="19" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
         <v>1</v>
       </c>
@@ -6091,22 +6091,22 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="G19" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>122</v>
+        <v>395</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6118,37 +6118,37 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W19" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="X19" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z19" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="X19" s="25" t="s">
-        <v>272</v>
-      </c>
-      <c r="Y19" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z19" s="25" t="s">
-        <v>276</v>
-      </c>
       <c r="AA19" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
         <v>1</v>
       </c>
@@ -6159,19 +6159,19 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6180,22 +6180,22 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6204,19 +6204,19 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="X20" s="25" t="s">
+      <c r="Y20" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA20" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="Y20" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="AA20" s="25" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="25">
         <v>1</v>
       </c>
@@ -6227,19 +6227,19 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F21" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H21" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6251,31 +6251,31 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y21" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
       <c r="AD21" s="25"/>
     </row>
-    <row r="22" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>1</v>
       </c>
@@ -6286,13 +6286,13 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>104</v>
@@ -6307,22 +6307,22 @@
         <v>2005</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M22" s="25">
         <v>0.1</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P22" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>290</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>291</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6331,25 +6331,25 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W22" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="X22" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y22" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z22" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="X22" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z22" s="25" t="s">
-        <v>293</v>
-      </c>
       <c r="AA22" s="25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="25">
         <v>1</v>
       </c>
@@ -6357,16 +6357,16 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>294</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>295</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>104</v>
@@ -6382,22 +6382,22 @@
         <v>2005</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M23" s="25">
         <v>0.1</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>296</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>297</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
@@ -6406,28 +6406,28 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W23" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="X23" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y23" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z23" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="X23" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y23" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z23" s="25" t="s">
-        <v>300</v>
-      </c>
       <c r="AA23" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB23" s="25"/>
       <c r="AC23" s="25"/>
       <c r="AD23" s="25"/>
     </row>
-    <row r="24" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>1</v>
       </c>
@@ -6435,22 +6435,22 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6460,58 +6460,58 @@
         <v>2005</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M24" s="25">
         <v>0.1</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>304</v>
-      </c>
       <c r="R24" s="25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S24" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="T24" s="25" t="s">
         <v>385</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>386</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="X24" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y24" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB24" s="25"/>
       <c r="AC24" s="25"/>
       <c r="AD24" s="25"/>
     </row>
-    <row r="25" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="25">
         <v>1</v>
       </c>
@@ -6519,16 +6519,16 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>306</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>307</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>104</v>
@@ -6544,58 +6544,58 @@
         <v>2005</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M25" s="25">
         <v>0.1</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>309</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>310</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W25" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="X25" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y25" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z25" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="X25" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z25" s="25" t="s">
-        <v>300</v>
-      </c>
       <c r="AA25" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB25" s="25"/>
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
     </row>
-    <row r="26" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="25">
         <v>1</v>
       </c>
@@ -6603,16 +6603,16 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>104</v>
@@ -6628,58 +6628,58 @@
         <v>2005</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M26" s="25">
         <v>0.1</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="R26" s="25" t="s">
-        <v>310</v>
-      </c>
       <c r="S26" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W26" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="X26" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y26" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="X26" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="Z26" s="25" t="s">
-        <v>300</v>
-      </c>
       <c r="AA26" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB26" s="25"/>
       <c r="AC26" s="25"/>
       <c r="AD26" s="25"/>
     </row>
-    <row r="27" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="25">
         <v>1</v>
       </c>
@@ -6687,22 +6687,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>314</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>315</v>
-      </c>
-      <c r="H27" t="s">
-        <v>316</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6712,14 +6712,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6727,32 +6727,32 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y27" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z27" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="Y27" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z27" s="25" t="s">
+      <c r="AA27" s="25" t="s">
         <v>322</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>323</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="25">
         <v>1</v>
       </c>
@@ -6760,41 +6760,41 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>325</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>326</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>327</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>328</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6805,27 +6805,27 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="25">
         <v>0</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6842,10 +6842,10 @@
         <v>88</v>
       </c>
       <c r="F29" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G29" s="34" t="s">
         <v>168</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>169</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>99</v>
@@ -6858,14 +6858,14 @@
         <v>2002</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6876,7 +6876,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6885,14 +6885,14 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
     </row>
-    <row r="30" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>1</v>
       </c>
@@ -6900,19 +6900,19 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F30" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" s="25" t="s">
         <v>168</v>
-      </c>
-      <c r="G30" s="25" t="s">
-        <v>169</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>102</v>
@@ -6927,16 +6927,16 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O30" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6945,25 +6945,25 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y30" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z30" s="25"/>
       <c r="AA30" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AB30" s="25"/>
       <c r="AC30" s="25"/>
       <c r="AD30" s="25"/>
       <c r="AE30" s="25"/>
     </row>
-    <row r="31" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="25">
         <v>1</v>
       </c>
@@ -6971,22 +6971,22 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>339</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>340</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6996,66 +6996,66 @@
         <v>2010</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M31" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="O31" s="25" t="s">
         <v>381</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="O31" s="25" t="s">
-        <v>382</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>341</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="X31" s="25" t="s">
-        <v>343</v>
-      </c>
       <c r="Y31" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="25">
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>344</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>345</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>314</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>315</v>
-      </c>
       <c r="H32" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7065,11 +7065,11 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O32" s="25"/>
       <c r="P32" s="30"/>
@@ -7081,10 +7081,10 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y32" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z32" s="25"/>
       <c r="AA32" s="25"/>
@@ -7092,7 +7092,7 @@
       <c r="AC32" s="25"/>
       <c r="AD32" s="25"/>
     </row>
-    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25">
         <v>1</v>
       </c>
@@ -7100,22 +7100,22 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>347</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>348</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F33" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H33" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7127,67 +7127,67 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Y33" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="25">
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>328</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7198,25 +7198,25 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
       <c r="AD34" s="25"/>
       <c r="AE34" s="25"/>
     </row>
-    <row r="35" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="25">
         <v>1</v>
       </c>
@@ -7233,13 +7233,13 @@
         <v>91</v>
       </c>
       <c r="F35" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H35" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7249,18 +7249,18 @@
         <v>2016</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M35" s="25"/>
       <c r="N35" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7269,25 +7269,25 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
     </row>
-    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25">
         <v>1</v>
       </c>
@@ -7304,13 +7304,13 @@
         <v>91</v>
       </c>
       <c r="F36" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>178</v>
-      </c>
       <c r="H36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7322,51 +7322,51 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Y36" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="25">
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="C37" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="D37" s="25" t="s">
+      <c r="E37" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I37" s="25" t="s">
         <v>361</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="I37" s="25" t="s">
-        <v>362</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7377,7 +7377,7 @@
       <c r="L37" s="25"/>
       <c r="M37" s="25"/>
       <c r="N37" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O37" s="25"/>
       <c r="P37" s="25"/>
@@ -7389,50 +7389,50 @@
         <v>115</v>
       </c>
       <c r="V37" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W37" s="25"/>
       <c r="X37" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y37" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="Y37" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="Z37" s="25"/>
       <c r="AA37" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB37" s="25"/>
       <c r="AC37" s="25"/>
       <c r="AD37" s="25"/>
     </row>
-    <row r="38" spans="1:31" ht="14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="25">
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="C38" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="D38" s="25" t="s">
+      <c r="E38" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I38" s="25" t="s">
         <v>364</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="G38" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>365</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7443,7 +7443,7 @@
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
       <c r="N38" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O38" s="25"/>
       <c r="P38" s="25"/>
@@ -7455,47 +7455,47 @@
         <v>115</v>
       </c>
       <c r="V38" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W38" s="25"/>
       <c r="X38" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y38" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="Y38" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="Z38" s="25"/>
       <c r="AA38" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB38" s="25"/>
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
     </row>
-    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25">
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="G39" t="s">
+        <v>177</v>
+      </c>
+      <c r="H39" t="s">
         <v>371</v>
-      </c>
-      <c r="G39" t="s">
-        <v>178</v>
-      </c>
-      <c r="H39" t="s">
-        <v>372</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7510,16 +7510,16 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>372</v>
+      </c>
+      <c r="X39" t="s">
         <v>373</v>
       </c>
-      <c r="X39" t="s">
-        <v>374</v>
-      </c>
       <c r="Y39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -7552,17 +7552,17 @@
     <hyperlink ref="G9" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
     <hyperlink ref="G16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
     <hyperlink ref="G17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G19" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="G32" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G18" r:id="rId36" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
+    <hyperlink ref="G32" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G14" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G34" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G2" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G36" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G37" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G38" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G18" r:id="rId35" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
+    <hyperlink ref="G19" r:id="rId36" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
@@ -7571,26 +7571,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7795,32 +7775,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7839,6 +7814,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{ab6d1c10-a186-47ab-af91-cdbff51004f3}" enabled="1" method="Standard" siteId="{a020d0ae-094a-4d44-b66c-ac3fe8e90c58}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
G4: new datasource and adapted computation
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD551CC8-81A2-47D8-B44A-83BAA6C17160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907EC0FA-4EEF-4D21-B76E-035174F3A872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,6 +64,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={8D6D4BDD-30EE-4AB7-91B4-A0AFA8CAA1BF}</author>
+    <author>tc={B959955C-40F8-4178-9D46-2B3B699FF6C4}</author>
     <author>tc={F8D71A7C-E5F7-4AB2-BA3A-263385823BB9}</author>
     <author>tc={AE0623BC-6FA4-49C9-B450-941BCEB6A906}</author>
   </authors>
@@ -76,7 +77,15 @@
     Titel der Grafiken</t>
       </text>
     </comment>
-    <comment ref="K20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{B959955C-40F8-4178-9D46-2B3B699FF6C4}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Ab 2025 aus OGD Datensatz MeteoSchweiz berechnet</t>
+      </text>
+    </comment>
+    <comment ref="K20" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -88,7 +97,7 @@
 Es wird die Anzahl Jahre abgefragt, also 2023-1996 = 27</t>
       </text>
     </comment>
-    <comment ref="H31" authorId="2" shapeId="0" xr:uid="{AE0623BC-6FA4-49C9-B450-941BCEB6A906}">
+    <comment ref="H31" authorId="3" shapeId="0" xr:uid="{AE0623BC-6FA4-49C9-B450-941BCEB6A906}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -746,21 +755,9 @@
     <t>Anzahl Heizgradtage pro Jahr</t>
   </si>
   <si>
-    <t>stadt zürich</t>
-  </si>
-  <si>
-    <t>https://www.stadt-zuerich.ch/content/dam/stzh/gud/Deutsch/UGZ/umwelt-energie/energie-in-zahlen/Heizgradtage/dokumente/</t>
-  </si>
-  <si>
-    <t>HGT%20Z%c3%bcrich_Fluntern_Monats_Jahreswerte_Zeitreihe_seit_1990.xlsx</t>
-  </si>
-  <si>
     <t>Heizgradtage (Jan-Dez)</t>
   </si>
   <si>
-    <t>Stadt Zürich, Gesundheits- und Umweltdepartement</t>
-  </si>
-  <si>
     <t xml:space="preserve">Installierte Leistung fossil betriebener Anlagen grösser 1 MW gemäss Grossfeuerungsdatenbank			</t>
   </si>
   <si>
@@ -1311,6 +1308,18 @@
   </si>
   <si>
     <t xml:space="preserve">Antriebsart bei neu beschafften Fahrzeugen der kantonalen Flotte </t>
+  </si>
+  <si>
+    <t>meteoschweiz</t>
+  </si>
+  <si>
+    <t>https://data.geo.admin.ch/ch.meteoschweiz.klima/nbcn-tageswerte/</t>
+  </si>
+  <si>
+    <t>nbcn-daily_SMA_previous.csv</t>
+  </si>
+  <si>
+    <t>Bundesamt für Meteorologie und Klimatologie MeteoSchweiz</t>
   </si>
 </sst>
 </file>
@@ -2084,7 +2093,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="12" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2173,6 +2182,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="20 % - Akzent1" xfId="42" builtinId="30" customBuiltin="1"/>
@@ -2702,6 +2712,9 @@
   <threadedComment ref="D1" dT="2023-06-14T07:18:41.28" personId="{808E65DB-4307-4BA3-BC76-03CCDC34E544}" id="{8D6D4BDD-30EE-4AB7-91B4-A0AFA8CAA1BF}">
     <text>Titel der Grafiken</text>
   </threadedComment>
+  <threadedComment ref="C9" dT="2025-01-16T12:30:30.52" personId="{9E374A6E-78EE-4895-9219-03BB83C00527}" id="{B959955C-40F8-4178-9D46-2B3B699FF6C4}">
+    <text>Ab 2025 aus OGD Datensatz MeteoSchweiz berechnet</text>
+  </threadedComment>
   <threadedComment ref="K20" dT="2023-05-03T08:29:37.28" personId="{808E65DB-4307-4BA3-BC76-03CCDC34E544}" id="{F8D71A7C-E5F7-4AB2-BA3A-263385823BB9}">
     <text>Jährliche Daten erst seit 1996 verfügbar, deshalb dort Start auch wenn erste Daten aus 1975 stammen.</text>
   </threadedComment>
@@ -4883,7 +4896,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5211,7 +5224,7 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
@@ -5309,10 +5322,10 @@
         <v>189</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5321,7 +5334,7 @@
         <v>190</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="W6" s="25" t="s">
         <v>191</v>
@@ -5483,23 +5496,23 @@
       <c r="D9" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>207</v>
+      <c r="E9" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>392</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>208</v>
+        <v>393</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>209</v>
+        <v>394</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
       </c>
       <c r="K9" s="25">
-        <v>1990</v>
+        <v>1864</v>
       </c>
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
@@ -5509,7 +5522,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5522,7 +5535,7 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>211</v>
+        <v>395</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>163</v>
@@ -5543,10 +5556,10 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
@@ -5558,7 +5571,7 @@
         <v>177</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5572,27 +5585,27 @@
         <v>179</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
@@ -5613,7 +5626,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
@@ -5643,31 +5656,31 @@
         <v>160</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="P11" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="U11" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="V11" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="W11" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="X11" s="25" t="s">
         <v>221</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="U11" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="V11" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="W11" s="35" t="s">
-        <v>224</v>
-      </c>
-      <c r="X11" s="25" t="s">
-        <v>225</v>
       </c>
       <c r="Y11" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z11" s="25" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>183</v>
@@ -5684,7 +5697,7 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
@@ -5696,7 +5709,7 @@
         <v>177</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5708,17 +5721,17 @@
         <v>179</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="U12" s="25" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5743,10 +5756,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
@@ -5755,13 +5768,13 @@
         <v>186</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5773,19 +5786,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="V13" s="25" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="X13" s="25" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5796,10 +5809,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5811,7 +5824,7 @@
         <v>177</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5821,28 +5834,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="U14" s="25" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="V14" s="25" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>163</v>
@@ -5862,19 +5875,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5886,26 +5899,26 @@
         <v>188</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="Q15" s="25" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="U15" s="25" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="V15" s="25" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>183</v>
@@ -5922,22 +5935,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5946,17 +5959,17 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="U16" s="25" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>163</v>
@@ -5979,19 +5992,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -6000,23 +6013,23 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="Q17" s="25" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="U17" s="25" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>175</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="Y17" s="25" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AA17" s="25" t="s">
         <v>205</v>
@@ -6033,10 +6046,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
@@ -6048,7 +6061,7 @@
         <v>168</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6057,20 +6070,20 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q18" s="25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="U18" s="25" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V18" s="25" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Y18" s="25" t="s">
         <v>181</v>
@@ -6091,10 +6104,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
@@ -6106,7 +6119,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6118,31 +6131,31 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W19" s="35" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="X19" s="25" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Y19" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>183</v>
@@ -6159,7 +6172,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
@@ -6171,7 +6184,7 @@
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6180,7 +6193,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6189,13 +6202,13 @@
         <v>160</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6204,16 +6217,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="X20" s="25" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6227,7 +6240,7 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
@@ -6239,7 +6252,7 @@
         <v>177</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6251,14 +6264,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6286,7 +6299,7 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
@@ -6316,13 +6329,13 @@
         <v>160</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P22" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="Q22" s="25" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6331,19 +6344,19 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W22" s="35" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="X22" s="25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="Y22" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AA22" s="25" t="s">
         <v>183</v>
@@ -6357,10 +6370,10 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
@@ -6391,13 +6404,13 @@
         <v>160</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="Q23" s="25" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
@@ -6406,19 +6419,19 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X23" s="25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="Y23" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AA23" s="25" t="s">
         <v>183</v>
@@ -6435,10 +6448,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -6450,7 +6463,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6469,40 +6482,40 @@
         <v>160</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P24" s="30" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="Q24" s="25" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="R24" s="25" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="S24" s="25" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="T24" s="25" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="X24" s="25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="Y24" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AA24" s="25" t="s">
         <v>183</v>
@@ -6519,10 +6532,10 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
@@ -6553,40 +6566,40 @@
         <v>160</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Q25" s="25" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W25" s="35" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X25" s="25" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AA25" s="25" t="s">
         <v>183</v>
@@ -6603,10 +6616,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
@@ -6637,40 +6650,40 @@
         <v>160</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="Q26" s="25" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="R26" s="25" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="S26" s="25" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="W26" s="35" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X26" s="25" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z26" s="25" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>183</v>
@@ -6687,22 +6700,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H27" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6712,14 +6725,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6727,29 +6740,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z27" s="25" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="AA27" s="25" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6760,32 +6773,32 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
@@ -6794,7 +6807,7 @@
         <v>179</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6805,14 +6818,14 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
@@ -6822,7 +6835,7 @@
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6833,7 +6846,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6865,7 +6878,7 @@
         <v>179</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6876,7 +6889,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6885,7 +6898,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6900,10 +6913,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6933,10 +6946,10 @@
         <v>170</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6945,7 +6958,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6971,10 +6984,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
@@ -6986,7 +6999,7 @@
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -6999,31 +7012,31 @@
         <v>188</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="V31" s="25" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="X31" s="25" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>163</v>
@@ -7037,25 +7050,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H32" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7065,7 +7078,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7081,7 +7094,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>163</v>
@@ -7100,10 +7113,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7115,7 +7128,7 @@
         <v>177</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7127,16 +7140,16 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>163</v>
@@ -7150,35 +7163,35 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
@@ -7187,7 +7200,7 @@
         <v>179</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7198,14 +7211,14 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
@@ -7239,7 +7252,7 @@
         <v>177</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7256,11 +7269,11 @@
         <v>179</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7269,14 +7282,14 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
@@ -7310,7 +7323,7 @@
         <v>177</v>
       </c>
       <c r="H36" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7322,16 +7335,16 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>163</v>
@@ -7345,13 +7358,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>155</v>
@@ -7366,7 +7379,7 @@
         <v>158</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7411,13 +7424,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>155</v>
@@ -7432,7 +7445,7 @@
         <v>158</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7477,25 +7490,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G39" t="s">
         <v>177</v>
       </c>
       <c r="H39" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7510,10 +7523,10 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="X39" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="Y39" t="s">
         <v>163</v>
@@ -7549,24 +7562,25 @@
     <hyperlink ref="G12" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
     <hyperlink ref="G15" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
     <hyperlink ref="G6" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="G9" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="G16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="G17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G32" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G18" r:id="rId35" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
-    <hyperlink ref="G19" r:id="rId36" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
+    <hyperlink ref="G16" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G17" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="G32" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G14" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G34" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G2" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G36" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G37" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G38" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G18" r:id="rId34" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
+    <hyperlink ref="G19" r:id="rId35" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
+    <hyperlink ref="G9" r:id="rId36" xr:uid="{45DBF95B-64C3-4D4C-AAA9-2A2D3E7DEB9B}"/>
+    <hyperlink ref="X9" r:id="rId37" display="https://opendata.swiss/de/organization/bundesamt-fur-meteorologie-und-klimatologie-meteoschweiz" xr:uid="{87CBCB47-9953-42A6-AE7D-A8BEBAC4E5C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
-  <legacyDrawing r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updating and adjustment of indicators EV1, EV2 and G2
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907EC0FA-4EEF-4D21-B76E-035174F3A872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2677AC05-4F02-4607-8419-F6E207D7FCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
     <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="395">
   <si>
     <t>#</t>
   </si>
@@ -717,9 +717,6 @@
   </si>
   <si>
     <t>Wärmegesamtverbrauch nach Energieträger</t>
-  </si>
-  <si>
-    <t>G2_data.csv</t>
   </si>
   <si>
     <t>Waerme</t>
@@ -2093,7 +2090,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="12" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2182,7 +2179,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="20 % - Akzent1" xfId="42" builtinId="30" customBuiltin="1"/>
@@ -4896,7 +4892,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5224,7 +5220,7 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
@@ -5322,10 +5318,10 @@
         <v>189</v>
       </c>
       <c r="P6" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q6" s="25" t="s">
         <v>372</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>373</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5334,7 +5330,7 @@
         <v>190</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W6" s="25" t="s">
         <v>191</v>
@@ -5372,13 +5368,13 @@
         <v>91</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>177</v>
+        <v>167</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>195</v>
+        <v>102</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>86</v>
@@ -5392,7 +5388,7 @@
         <v>179</v>
       </c>
       <c r="O7" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q7" s="25" t="s">
         <v>180</v>
@@ -5414,10 +5410,13 @@
         <v>163</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>183</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5431,7 +5430,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
@@ -5443,10 +5442,10 @@
         <v>177</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>199</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>200</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
@@ -5456,31 +5455,31 @@
         <v>179</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>203</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5494,19 +5493,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>393</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>394</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5522,7 +5521,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5535,14 +5534,14 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
@@ -5556,10 +5555,10 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>208</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>209</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
@@ -5571,7 +5570,7 @@
         <v>177</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5585,31 +5584,31 @@
         <v>179</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
@@ -5626,7 +5625,7 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
@@ -5656,31 +5655,31 @@
         <v>160</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="W11" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="V11" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="W11" s="35" t="s">
+      <c r="X11" s="25" t="s">
         <v>220</v>
-      </c>
-      <c r="X11" s="25" t="s">
-        <v>221</v>
       </c>
       <c r="Y11" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z11" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>183</v>
@@ -5697,7 +5696,7 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
@@ -5709,7 +5708,7 @@
         <v>177</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5721,17 +5720,17 @@
         <v>179</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="U12" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>225</v>
-      </c>
-      <c r="U12" s="25" t="s">
-        <v>363</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>226</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5742,7 +5741,7 @@
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -5756,10 +5755,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>227</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>228</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
@@ -5768,13 +5767,13 @@
         <v>186</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>230</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>231</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5786,19 +5785,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>233</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5809,10 +5808,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5824,7 +5823,7 @@
         <v>177</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5834,28 +5833,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>241</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>163</v>
@@ -5875,19 +5874,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5899,26 +5898,26 @@
         <v>188</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="U15" s="25" t="s">
-        <v>247</v>
-      </c>
       <c r="V15" s="25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>183</v>
@@ -5935,22 +5934,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>360</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>361</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5959,23 +5958,23 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>252</v>
       </c>
-      <c r="U16" s="25" t="s">
-        <v>253</v>
-      </c>
       <c r="V16" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -5992,19 +5991,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -6013,26 +6012,26 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>258</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>259</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>175</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="Y17" s="25" t="s">
-        <v>261</v>
-      </c>
       <c r="AA17" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -6046,10 +6045,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>263</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
@@ -6061,7 +6060,7 @@
         <v>168</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6070,20 +6069,20 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>265</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y18" s="25" t="s">
         <v>181</v>
@@ -6104,10 +6103,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
@@ -6119,7 +6118,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6131,31 +6130,31 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W19" s="35" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X19" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y19" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z19" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>183</v>
@@ -6172,7 +6171,7 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
@@ -6184,7 +6183,7 @@
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6193,7 +6192,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6202,13 +6201,13 @@
         <v>160</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6217,16 +6216,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>276</v>
-      </c>
-      <c r="X20" s="25" t="s">
-        <v>277</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6240,7 +6239,7 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
@@ -6252,7 +6251,7 @@
         <v>177</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6264,14 +6263,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6282,7 +6281,7 @@
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
@@ -6299,7 +6298,7 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
@@ -6329,13 +6328,13 @@
         <v>160</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P22" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>284</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>285</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6344,19 +6343,19 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W22" s="35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="X22" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y22" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z22" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AA22" s="25" t="s">
         <v>183</v>
@@ -6370,10 +6369,10 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>288</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>289</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
@@ -6404,13 +6403,13 @@
         <v>160</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>290</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>291</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
@@ -6419,19 +6418,19 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W23" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X23" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y23" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z23" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA23" s="25" t="s">
         <v>183</v>
@@ -6448,10 +6447,10 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -6463,7 +6462,7 @@
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6482,40 +6481,40 @@
         <v>160</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>298</v>
-      </c>
       <c r="R24" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S24" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="T24" s="25" t="s">
         <v>379</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>380</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="X24" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y24" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA24" s="25" t="s">
         <v>183</v>
@@ -6532,10 +6531,10 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>300</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>301</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
@@ -6566,40 +6565,40 @@
         <v>160</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>303</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>304</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W25" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X25" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z25" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA25" s="25" t="s">
         <v>183</v>
@@ -6616,10 +6615,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
@@ -6650,40 +6649,40 @@
         <v>160</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="R26" s="25" t="s">
-        <v>304</v>
-      </c>
       <c r="S26" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W26" s="35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X26" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Y26" s="25" t="s">
         <v>181</v>
       </c>
       <c r="Z26" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>183</v>
@@ -6700,22 +6699,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>309</v>
-      </c>
-      <c r="H27" t="s">
-        <v>310</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6725,14 +6724,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6740,29 +6739,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>313</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>314</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z27" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA27" s="25" t="s">
         <v>316</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>317</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6773,32 +6772,32 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>319</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>320</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>321</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>322</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
@@ -6807,7 +6806,7 @@
         <v>179</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6818,24 +6817,24 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6846,7 +6845,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6878,7 +6877,7 @@
         <v>179</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6889,7 +6888,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6898,7 +6897,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6913,10 +6912,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6946,10 +6945,10 @@
         <v>170</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6958,7 +6957,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6984,10 +6983,10 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>333</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>334</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
@@ -6999,7 +6998,7 @@
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -7012,37 +7011,37 @@
         <v>188</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>336</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -7050,25 +7049,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>338</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>339</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="H32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7078,7 +7077,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7094,7 +7093,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>163</v>
@@ -7113,10 +7112,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>341</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>342</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7128,7 +7127,7 @@
         <v>177</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7140,22 +7139,22 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -7163,35 +7162,35 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>322</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
@@ -7200,7 +7199,7 @@
         <v>179</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7211,18 +7210,18 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
@@ -7252,7 +7251,7 @@
         <v>177</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7269,11 +7268,11 @@
         <v>179</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7282,18 +7281,18 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
@@ -7323,7 +7322,7 @@
         <v>177</v>
       </c>
       <c r="H36" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7335,22 +7334,22 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -7358,13 +7357,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>155</v>
@@ -7379,7 +7378,7 @@
         <v>158</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7424,13 +7423,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>155</v>
@@ -7445,7 +7444,7 @@
         <v>158</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7490,25 +7489,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G39" t="s">
         <v>177</v>
       </c>
       <c r="H39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7523,16 +7522,16 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>366</v>
+      </c>
+      <c r="X39" t="s">
         <v>367</v>
-      </c>
-      <c r="X39" t="s">
-        <v>368</v>
       </c>
       <c r="Y39" t="s">
         <v>163</v>
       </c>
       <c r="AA39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -7557,26 +7556,26 @@
     <hyperlink ref="G10" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
     <hyperlink ref="G8" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
     <hyperlink ref="G5" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="G7" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="G21" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="G12" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="G15" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="G6" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="G16" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="G17" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G32" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G18" r:id="rId34" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
-    <hyperlink ref="G19" r:id="rId35" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
-    <hyperlink ref="G9" r:id="rId36" xr:uid="{45DBF95B-64C3-4D4C-AAA9-2A2D3E7DEB9B}"/>
-    <hyperlink ref="X9" r:id="rId37" display="https://opendata.swiss/de/organization/bundesamt-fur-meteorologie-und-klimatologie-meteoschweiz" xr:uid="{87CBCB47-9953-42A6-AE7D-A8BEBAC4E5C9}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G15" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="G6" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G16" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G17" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="G32" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G14" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G34" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G2" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G36" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G37" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G38" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G18" r:id="rId33" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
+    <hyperlink ref="G19" r:id="rId34" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
+    <hyperlink ref="G9" r:id="rId35" xr:uid="{45DBF95B-64C3-4D4C-AAA9-2A2D3E7DEB9B}"/>
+    <hyperlink ref="X9" r:id="rId36" display="https://opendata.swiss/de/organization/bundesamt-fur-meteorologie-und-klimatologie-meteoschweiz" xr:uid="{87CBCB47-9953-42A6-AE7D-A8BEBAC4E5C9}"/>
+    <hyperlink ref="G7" r:id="rId37" xr:uid="{E38DCCD6-5095-472B-97C6-7079C8648A62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
@@ -7585,6 +7584,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
@@ -7593,15 +7601,6 @@
     <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7810,6 +7809,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -7822,14 +7829,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating and adjustment of indicator EV3
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2677AC05-4F02-4607-8419-F6E207D7FCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0C20D5-78D9-4235-97EF-65B7B8AF9BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="394">
   <si>
     <t>#</t>
   </si>
@@ -666,9 +666,6 @@
   </si>
   <si>
     <t>https://www.web.statistik.zh.ch/awel/decarb_monitoring/</t>
-  </si>
-  <si>
-    <t>EV3_data.csv</t>
   </si>
   <si>
     <t>Zürich</t>
@@ -4889,10 +4886,10 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5220,19 +5217,19 @@
         <v>117</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>177</v>
+        <v>167</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>86</v>
@@ -5242,13 +5239,13 @@
       </c>
       <c r="L5" s="25"/>
       <c r="N5" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O5" s="25" t="s">
         <v>175</v>
       </c>
       <c r="Q5" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
@@ -5264,13 +5261,16 @@
         <v>101</v>
       </c>
       <c r="Y5" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z5" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="AA5" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="AA5" s="25" t="s">
-        <v>183</v>
+      <c r="AE5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5281,22 +5281,22 @@
         <v>53</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>184</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>185</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="34" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25" t="s">
@@ -5306,7 +5306,7 @@
         <v>2021</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M6" s="25">
         <v>0.1</v>
@@ -5315,37 +5315,37 @@
         <v>160</v>
       </c>
       <c r="O6" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P6" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q6" s="25" t="s">
         <v>371</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>372</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
       <c r="U6" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="V6" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="W6" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="V6" s="25" t="s">
-        <v>387</v>
-      </c>
-      <c r="W6" s="25" t="s">
+      <c r="X6" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="Y6" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z6" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="Y6" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z6" s="32" t="s">
-        <v>193</v>
-      </c>
       <c r="AA6" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
@@ -5362,7 +5362,7 @@
         <v>89</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>91</v>
@@ -5385,13 +5385,13 @@
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
       <c r="N7" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>180</v>
       </c>
       <c r="R7" s="25"/>
       <c r="S7" s="25"/>
@@ -5410,10 +5410,10 @@
         <v>163</v>
       </c>
       <c r="Z7" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AA7" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AE7" t="s">
         <v>74</v>
@@ -5430,7 +5430,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>91</v>
@@ -5442,44 +5442,44 @@
         <v>177</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>199</v>
       </c>
       <c r="K8" s="25">
         <v>1990</v>
       </c>
       <c r="L8" s="25"/>
       <c r="N8" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P8" s="25"/>
       <c r="Q8" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R8" s="25"/>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="V8" s="25" t="s">
         <v>201</v>
-      </c>
-      <c r="V8" s="25" t="s">
-        <v>202</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y8" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -5493,19 +5493,19 @@
         <v>92</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>392</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>393</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5516,12 +5516,12 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R9" s="25"/>
       <c r="S9" s="25"/>
@@ -5534,14 +5534,14 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z9" s="25"/>
       <c r="AA9" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="25"/>
@@ -5555,10 +5555,10 @@
         <v>65</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>207</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>208</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
@@ -5570,7 +5570,7 @@
         <v>177</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5581,34 +5581,34 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P10" s="30"/>
       <c r="Q10" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="25" t="s">
         <v>101</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z10" s="25"/>
       <c r="AA10" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB10" s="25"/>
       <c r="AC10" s="25"/>
@@ -5625,13 +5625,13 @@
         <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>104</v>
@@ -5646,7 +5646,7 @@
         <v>2005</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M11" s="25">
         <v>0.1</v>
@@ -5655,34 +5655,34 @@
         <v>160</v>
       </c>
       <c r="O11" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="P11" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="Q11" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="U11" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="V11" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="W11" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="V11" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="W11" s="35" t="s">
+      <c r="X11" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="X11" s="25" t="s">
+      <c r="Y11" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z11" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="Y11" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z11" s="25" t="s">
-        <v>221</v>
-      </c>
       <c r="AA11" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5696,7 +5696,7 @@
         <v>107</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>91</v>
@@ -5708,7 +5708,7 @@
         <v>177</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5717,20 +5717,20 @@
         <v>2020</v>
       </c>
       <c r="N12" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P12"/>
       <c r="Q12" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="U12" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="V12" s="25" t="s">
         <v>224</v>
-      </c>
-      <c r="U12" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>225</v>
       </c>
       <c r="W12"/>
       <c r="X12" s="25" t="s">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="Z12"/>
       <c r="AA12" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB12"/>
       <c r="AC12"/>
@@ -5755,25 +5755,25 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>226</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>227</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>229</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>230</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>86</v>
@@ -5785,19 +5785,19 @@
         <v>85</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="V13" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="X13" s="25" t="s">
         <v>231</v>
-      </c>
-      <c r="X13" s="25" t="s">
-        <v>232</v>
       </c>
       <c r="Y13" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA13" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -5808,10 +5808,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>91</v>
@@ -5823,7 +5823,7 @@
         <v>177</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="25" t="s">
@@ -5833,28 +5833,28 @@
         <v>2007</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M14"/>
       <c r="N14" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P14"/>
       <c r="Q14" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="U14" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="U14" s="25" t="s">
-        <v>240</v>
-      </c>
       <c r="V14" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="W14"/>
       <c r="X14" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Y14" s="25" t="s">
         <v>163</v>
@@ -5874,19 +5874,19 @@
         <v>118</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>86</v>
@@ -5895,32 +5895,32 @@
         <v>2021</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q15" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="U15" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="U15" s="25" t="s">
-        <v>246</v>
-      </c>
       <c r="V15" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W15"/>
       <c r="X15" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y15" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z15" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AA15" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB15"/>
       <c r="AC15"/>
@@ -5934,22 +5934,22 @@
         <v>81</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>359</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>360</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>86</v>
@@ -5958,23 +5958,23 @@
         <v>2011</v>
       </c>
       <c r="O16" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="U16" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="U16" s="25" t="s">
-        <v>252</v>
-      </c>
       <c r="V16" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Y16" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA16" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB16"/>
       <c r="AC16"/>
@@ -5991,19 +5991,19 @@
         <v>121</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>177</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>86</v>
@@ -6012,26 +6012,26 @@
         <v>2010</v>
       </c>
       <c r="O17" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="Q17" s="25" t="s">
+      <c r="U17" s="25" t="s">
         <v>257</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>258</v>
       </c>
       <c r="V17" s="25" t="s">
         <v>175</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y17" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="Y17" s="25" t="s">
-        <v>260</v>
-      </c>
       <c r="AA17" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB17"/>
       <c r="AC17"/>
@@ -6045,10 +6045,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>261</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>262</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>91</v>
@@ -6060,7 +6060,7 @@
         <v>168</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>86</v>
@@ -6069,27 +6069,27 @@
         <v>2015</v>
       </c>
       <c r="O18" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q18" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="Q18" s="25" t="s">
+      <c r="U18" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="V18" s="25" t="s">
         <v>264</v>
-      </c>
-      <c r="U18" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="V18" s="25" t="s">
-        <v>265</v>
       </c>
       <c r="W18"/>
       <c r="X18" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Y18" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z18"/>
       <c r="AA18" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB18"/>
       <c r="AC18"/>
@@ -6103,10 +6103,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>91</v>
@@ -6118,7 +6118,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6130,34 +6130,34 @@
         <v>93</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="R19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U19" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V19" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W19" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="X19" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y19" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z19" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="X19" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="Y19" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z19" s="25" t="s">
-        <v>269</v>
-      </c>
       <c r="AA19" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6171,19 +6171,19 @@
         <v>109</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6192,7 +6192,7 @@
         <v>1996</v>
       </c>
       <c r="L20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M20" s="25">
         <v>1.2</v>
@@ -6201,13 +6201,13 @@
         <v>160</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P20">
         <v>16</v>
       </c>
       <c r="Q20" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
@@ -6216,16 +6216,16 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="X20" s="25" t="s">
         <v>275</v>
-      </c>
-      <c r="X20" s="25" t="s">
-        <v>276</v>
       </c>
       <c r="Y20" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA20" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6239,7 +6239,7 @@
         <v>110</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>91</v>
@@ -6251,7 +6251,7 @@
         <v>177</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>86</v>
@@ -6263,14 +6263,14 @@
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P21" s="25"/>
       <c r="U21" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25" t="s">
@@ -6281,7 +6281,7 @@
       </c>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB21" s="25"/>
       <c r="AC21" s="25"/>
@@ -6298,13 +6298,13 @@
         <v>112</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>104</v>
@@ -6319,7 +6319,7 @@
         <v>2005</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M22" s="25">
         <v>0.1</v>
@@ -6328,13 +6328,13 @@
         <v>160</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P22" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>283</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>284</v>
       </c>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
@@ -6343,22 +6343,22 @@
         <v>93</v>
       </c>
       <c r="V22" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W22" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="X22" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y22" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z22" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="X22" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z22" s="25" t="s">
-        <v>286</v>
-      </c>
       <c r="AA22" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -6369,16 +6369,16 @@
         <v>57</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>287</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>288</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>104</v>
@@ -6394,7 +6394,7 @@
         <v>2005</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M23" s="25">
         <v>0.1</v>
@@ -6403,13 +6403,13 @@
         <v>160</v>
       </c>
       <c r="O23" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P23" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q23" s="25" t="s">
         <v>289</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>290</v>
       </c>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
@@ -6418,22 +6418,22 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W23" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="X23" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y23" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z23" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="X23" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="Y23" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z23" s="25" t="s">
-        <v>293</v>
-      </c>
       <c r="AA23" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB23" s="25"/>
       <c r="AC23" s="25"/>
@@ -6447,22 +6447,22 @@
         <v>58</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G24" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6472,7 +6472,7 @@
         <v>2005</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M24" s="25">
         <v>0.1</v>
@@ -6481,43 +6481,43 @@
         <v>160</v>
       </c>
       <c r="O24" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P24" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q24" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="Q24" s="25" t="s">
-        <v>297</v>
-      </c>
       <c r="R24" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S24" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="T24" s="25" t="s">
         <v>378</v>
-      </c>
-      <c r="T24" s="25" t="s">
-        <v>379</v>
       </c>
       <c r="U24" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W24" s="35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X24" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y24" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB24" s="25"/>
       <c r="AC24" s="25"/>
@@ -6531,16 +6531,16 @@
         <v>59</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>299</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>300</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>104</v>
@@ -6556,7 +6556,7 @@
         <v>2005</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M25" s="25">
         <v>0.1</v>
@@ -6565,43 +6565,43 @@
         <v>160</v>
       </c>
       <c r="O25" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P25" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="Q25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>302</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>303</v>
       </c>
       <c r="S25" s="25">
         <v>100</v>
       </c>
       <c r="T25" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W25" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="X25" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y25" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z25" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="X25" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z25" s="25" t="s">
-        <v>293</v>
-      </c>
       <c r="AA25" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB25" s="25"/>
       <c r="AC25" s="25"/>
@@ -6615,16 +6615,16 @@
         <v>60</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G26" s="34" t="s">
         <v>104</v>
@@ -6640,7 +6640,7 @@
         <v>2005</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M26" s="25">
         <v>0.1</v>
@@ -6649,43 +6649,43 @@
         <v>160</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P26" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q26" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="Q26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="R26" s="25" t="s">
-        <v>303</v>
-      </c>
       <c r="S26" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="T26" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W26" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="X26" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y26" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z26" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="X26" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z26" s="25" t="s">
-        <v>293</v>
-      </c>
       <c r="AA26" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB26" s="25"/>
       <c r="AC26" s="25"/>
@@ -6699,22 +6699,22 @@
         <v>61</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>307</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="H27" t="s">
         <v>308</v>
-      </c>
-      <c r="H27" t="s">
-        <v>309</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6724,14 +6724,14 @@
         <v>2014</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M27" s="25"/>
       <c r="N27" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O27" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P27" s="30"/>
       <c r="Q27" s="25"/>
@@ -6739,29 +6739,29 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="V27" s="25" t="s">
         <v>312</v>
-      </c>
-      <c r="V27" s="25" t="s">
-        <v>313</v>
       </c>
       <c r="W27" s="25"/>
       <c r="X27" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y27" s="25" t="s">
         <v>163</v>
       </c>
       <c r="Z27" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA27" s="25" t="s">
         <v>315</v>
-      </c>
-      <c r="AA27" s="25" t="s">
-        <v>316</v>
       </c>
       <c r="AB27" s="25"/>
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
       <c r="AE27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6772,41 +6772,41 @@
         <v>62</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>318</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>319</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="G28" s="34" t="s">
         <v>320</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>321</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K28" s="25">
         <v>2013</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M28" s="25">
         <v>0</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O28" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P28" s="25"/>
       <c r="Q28" s="25"/>
@@ -6817,24 +6817,24 @@
         <v>87</v>
       </c>
       <c r="V28" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W28" s="25"/>
       <c r="X28" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y28" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z28" s="25"/>
       <c r="AA28" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB28" s="25"/>
       <c r="AC28" s="25"/>
       <c r="AD28" s="25"/>
       <c r="AE28" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -6845,7 +6845,7 @@
         <v>63</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>98</v>
@@ -6870,14 +6870,14 @@
         <v>2002</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M29" s="25"/>
       <c r="N29" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
@@ -6888,7 +6888,7 @@
         <v>93</v>
       </c>
       <c r="V29" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="W29" s="25"/>
       <c r="X29" s="25" t="s">
@@ -6897,7 +6897,7 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
       <c r="AA29" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AB29" s="25"/>
       <c r="AC29" s="25"/>
@@ -6912,10 +6912,10 @@
         <v>64</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>91</v>
@@ -6939,16 +6939,16 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
       <c r="N30" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O30" s="25" t="s">
         <v>170</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q30" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
@@ -6957,7 +6957,7 @@
         <v>100</v>
       </c>
       <c r="V30" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="W30" s="25"/>
       <c r="X30" s="25" t="s">
@@ -6983,22 +6983,22 @@
         <v>52</v>
       </c>
       <c r="C31" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>332</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>333</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>104</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25" t="s">
@@ -7008,40 +7008,40 @@
         <v>2010</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N31" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O31" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="P31" s="25">
         <v>1</v>
       </c>
       <c r="Q31" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="V31" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="V31" s="25" t="s">
+      <c r="X31" s="25" t="s">
         <v>335</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>336</v>
       </c>
       <c r="Y31" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA31" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="15" x14ac:dyDescent="0.2">
@@ -7049,25 +7049,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C32" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>337</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>338</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F32" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="G32" s="33" t="s">
         <v>307</v>
       </c>
-      <c r="G32" s="33" t="s">
-        <v>308</v>
-      </c>
       <c r="H32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7077,7 +7077,7 @@
         <v>2014</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M32" s="25"/>
       <c r="N32" s="25" t="s">
@@ -7093,7 +7093,7 @@
       <c r="V32" s="25"/>
       <c r="W32" s="25"/>
       <c r="X32" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>163</v>
@@ -7112,10 +7112,10 @@
         <v>69</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>340</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>341</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7127,7 +7127,7 @@
         <v>177</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>86</v>
@@ -7139,22 +7139,22 @@
         <v>85</v>
       </c>
       <c r="O33" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="U33" s="25" t="s">
         <v>87</v>
       </c>
       <c r="V33" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X33" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="Y33" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA33" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
@@ -7162,44 +7162,44 @@
         <v>1</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>91</v>
       </c>
       <c r="F34" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>321</v>
-      </c>
       <c r="H34" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I34" s="25"/>
       <c r="J34" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K34" s="25">
         <v>2013</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M34" s="25">
         <v>0</v>
       </c>
       <c r="N34" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>
@@ -7210,18 +7210,18 @@
         <v>87</v>
       </c>
       <c r="V34" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W34" s="25"/>
       <c r="X34" s="25" t="s">
         <v>96</v>
       </c>
       <c r="Y34" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB34" s="25"/>
       <c r="AC34" s="25"/>
@@ -7251,7 +7251,7 @@
         <v>177</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7261,18 +7261,18 @@
         <v>2016</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M35" s="25"/>
       <c r="N35" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O35" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P35" s="25"/>
       <c r="Q35" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
@@ -7281,18 +7281,18 @@
         <v>108</v>
       </c>
       <c r="V35" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W35" s="25"/>
       <c r="X35" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Y35" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z35" s="25"/>
       <c r="AA35" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB35" s="25"/>
       <c r="AC35" s="25"/>
@@ -7322,7 +7322,7 @@
         <v>177</v>
       </c>
       <c r="H36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J36" t="s">
         <v>86</v>
@@ -7334,22 +7334,22 @@
         <v>85</v>
       </c>
       <c r="O36" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U36" t="s">
         <v>87</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X36" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>163</v>
       </c>
       <c r="AA36" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
@@ -7357,13 +7357,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>155</v>
@@ -7378,7 +7378,7 @@
         <v>158</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>86</v>
@@ -7423,13 +7423,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>153</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>155</v>
@@ -7444,7 +7444,7 @@
         <v>158</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7489,25 +7489,25 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G39" t="s">
         <v>177</v>
       </c>
       <c r="H39" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J39" t="s">
         <v>86</v>
@@ -7522,16 +7522,16 @@
         <v>93</v>
       </c>
       <c r="V39" t="s">
+        <v>365</v>
+      </c>
+      <c r="X39" t="s">
         <v>366</v>
-      </c>
-      <c r="X39" t="s">
-        <v>367</v>
       </c>
       <c r="Y39" t="s">
         <v>163</v>
       </c>
       <c r="AA39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -7555,27 +7555,27 @@
     <hyperlink ref="G4" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
     <hyperlink ref="G10" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
     <hyperlink ref="G8" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="G5" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="G21" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="G15" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="G6" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="G16" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="G17" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G32" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="G33" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G14" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="G34" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G2" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="G35" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G36" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="G37" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G38" r:id="rId32" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="G18" r:id="rId33" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
-    <hyperlink ref="G19" r:id="rId34" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
-    <hyperlink ref="G9" r:id="rId35" xr:uid="{45DBF95B-64C3-4D4C-AAA9-2A2D3E7DEB9B}"/>
-    <hyperlink ref="X9" r:id="rId36" display="https://opendata.swiss/de/organization/bundesamt-fur-meteorologie-und-klimatologie-meteoschweiz" xr:uid="{87CBCB47-9953-42A6-AE7D-A8BEBAC4E5C9}"/>
-    <hyperlink ref="G7" r:id="rId37" xr:uid="{E38DCCD6-5095-472B-97C6-7079C8648A62}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="G12" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G15" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="G6" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G16" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G17" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="G32" r:id="rId23" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId24" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="G14" r:id="rId25" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G34" r:id="rId26" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="G2" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G35" r:id="rId28" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="G36" r:id="rId29" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G37" r:id="rId30" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="G38" r:id="rId31" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G18" r:id="rId32" xr:uid="{08A8D72E-5F85-4B6D-A60B-BE57DB47A4B9}"/>
+    <hyperlink ref="G19" r:id="rId33" xr:uid="{FFA6C1C0-40AD-41E8-B332-030C91F94D32}"/>
+    <hyperlink ref="G9" r:id="rId34" xr:uid="{45DBF95B-64C3-4D4C-AAA9-2A2D3E7DEB9B}"/>
+    <hyperlink ref="X9" r:id="rId35" display="https://opendata.swiss/de/organization/bundesamt-fur-meteorologie-und-klimatologie-meteoschweiz" xr:uid="{87CBCB47-9953-42A6-AE7D-A8BEBAC4E5C9}"/>
+    <hyperlink ref="G7" r:id="rId36" xr:uid="{E38DCCD6-5095-472B-97C6-7079C8648A62}"/>
+    <hyperlink ref="G5" r:id="rId37" xr:uid="{4F90DBEB-F688-426E-9D75-B0CD71EAA2D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
@@ -7584,15 +7584,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
@@ -7601,6 +7592,15 @@
     <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7809,14 +7809,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -7829,6 +7821,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
A2/KG3/LF1 updated with new data
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAD4601-6CB6-4B3A-AF1C-0F9C65F3DF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83198D8C-4C2D-44E3-906B-2DFF92FFA088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17640" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1331,10 +1331,10 @@
     <t>Feuerungen [Anz.]</t>
   </si>
   <si>
-    <t>1: Oel, 2: Gas</t>
-  </si>
-  <si>
     <t>Anzahl fossil betriebene Feuerungen</t>
+  </si>
+  <si>
+    <t>Oel, Gas</t>
   </si>
 </sst>
 </file>
@@ -4915,10 +4915,10 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5587,7 +5587,7 @@
         <v>395</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>91</v>
@@ -5630,8 +5630,8 @@
       <c r="V10" s="25" t="s">
         <v>398</v>
       </c>
-      <c r="W10" s="37" t="s">
-        <v>399</v>
+      <c r="W10" s="25" t="s">
+        <v>400</v>
       </c>
       <c r="X10" s="25" t="s">
         <v>101</v>
@@ -6302,7 +6302,7 @@
         <v>272</v>
       </c>
       <c r="P21">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>273</v>
@@ -7683,26 +7683,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7907,32 +7887,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7951,6 +7926,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{ab6d1c10-a186-47ab-af91-cdbff51004f3}" enabled="1" method="Standard" siteId="{a020d0ae-094a-4d44-b66c-ac3fe8e90c58}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Updated output data for G5 - new titel and unit label
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corinna.grobe@zh.ch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A21358-D9BD-4BBF-9C20-9B35E970D318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08139977-3A44-4E66-A232-523D4CC1A1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17520" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -4915,10 +4915,10 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5624,8 +5624,8 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
-      <c r="U10" s="25" t="s">
-        <v>93</v>
+      <c r="U10" s="31" t="s">
+        <v>400</v>
       </c>
       <c r="V10" s="25" t="s">
         <v>397</v>
@@ -7683,17 +7683,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7898,6 +7887,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7908,23 +7908,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7943,6 +7926,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fix: description & xlsx
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\zz_tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp.bosch@zh.ch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA19A67B-36F9-4004-8726-0AD34C6950C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8461F03B-A791-4DF1-A959-80054ED08509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17520" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostenübersicht" sheetId="51" state="hidden" r:id="rId1"/>
@@ -35,14 +35,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
+    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
+    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
+    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
+    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
     <customWorkbookView name="Basil Odermatt - Persönliche Ansicht" guid="{59C26AB4-86C6-4447-8F9F-F1FCBFE3A683}" mergeInterval="0" personalView="1" maximized="1" xWindow="2552" yWindow="-6" windowWidth="2576" windowHeight="1426" activeSheetId="1"/>
-    <customWorkbookView name="Andrea Binkert - Persönliche Ansicht" guid="{2A6B7D3A-520D-4798-8230-1DC17916761C}" mergeInterval="0" personalView="1" xWindow="492" windowWidth="948" windowHeight="860" activeSheetId="1"/>
-    <customWorkbookView name="Dmoos - Persönliche Ansicht" guid="{D178FE1B-3B10-414B-86B8-943130264B26}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Urs Müller - Persönliche Ansicht" guid="{684E191D-B776-4614-A9A6-09F48EE40BD1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="978" activeSheetId="1"/>
-    <customWorkbookView name="Ernst Haas - Persönliche Ansicht" guid="{E9B280C6-F6C1-4D6E-A20C-7C4266B3269C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="923" activeSheetId="1"/>
-    <customWorkbookView name="Daniel Moos - Persönliche Ansicht" guid="{9D53A792-EE49-4CB1-A328-80A3B1745755}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1216" activeSheetId="1" showComments="commNone"/>
-    <customWorkbookView name="w10 Test - Persönliche Ansicht" guid="{F0C3F358-38F8-4A2B-A44F-0486E20EA4EB}" mergeInterval="0" personalView="1" xWindow="153" yWindow="43" windowWidth="1713" windowHeight="1088" activeSheetId="1"/>
-    <customWorkbookView name="Reto Dettli - Persönliche Ansicht" guid="{EFCCBDBE-703D-49A8-BFD5-C70DFC4C6246}" mergeInterval="0" personalView="1" maximized="1" xWindow="182" yWindow="-1449" windowWidth="2578" windowHeight="1398" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="402">
   <si>
     <t>#</t>
   </si>
@@ -1241,9 +1241,6 @@
     <t>Gesamtstromverbrauch</t>
   </si>
   <si>
-    <t>0,1,2,3,4,5,6,7,8</t>
-  </si>
-  <si>
     <t>Heizöl,Gas,Wärmepumpe,Holz,Elektrizität,Fernwärme,Sonne (thermisch),Andere,Keine</t>
   </si>
   <si>
@@ -1346,13 +1343,10 @@
     <t>8100+ZH</t>
   </si>
   <si>
-    <t>A._T._T.._T.</t>
-  </si>
-  <si>
     <t>https://disseminate.stats.swiss/rest/data/</t>
   </si>
   <si>
-    <t>CH1.GWS,DF_GWS_REG4,1.0.0/</t>
+    <t>CH1.GWS,DF_GWS_REG4,1.0.0/A._T._T.._T.</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1361,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; CHF&quot;"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -1648,12 +1642,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="45">
@@ -2138,7 +2126,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="12" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2229,9 +2217,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="42" borderId="0" xfId="8" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="20 % - Akzent1" xfId="42" builtinId="30" customBuiltin="1"/>
@@ -2802,24 +2787,24 @@
       <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="124.1640625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.1640625" style="2"/>
-    <col min="6" max="6" width="16.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.1640625" style="2"/>
-    <col min="13" max="13" width="15.1640625" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.1640625" style="2"/>
-    <col min="16" max="17" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.1640625" style="2"/>
+    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="124.109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.109375" style="2"/>
+    <col min="6" max="6" width="16.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="10.109375" style="2"/>
+    <col min="13" max="13" width="15.109375" style="2" customWidth="1"/>
+    <col min="14" max="15" width="10.109375" style="2"/>
+    <col min="16" max="17" width="17.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:11" ht="104.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" ht="103.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2854,7 +2839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>1.01</v>
       </c>
@@ -2899,7 +2884,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>1.02</v>
       </c>
@@ -2944,7 +2929,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>1.03</v>
       </c>
@@ -2989,7 +2974,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1.04</v>
       </c>
@@ -3034,7 +3019,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -3079,7 +3064,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +3109,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
@@ -3169,7 +3154,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -3214,7 +3199,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -3259,7 +3244,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -3304,7 +3289,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -3349,7 +3334,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>18</v>
       </c>
@@ -3394,7 +3379,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
@@ -3439,7 +3424,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
@@ -3484,7 +3469,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
@@ -3529,7 +3514,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
@@ -3574,7 +3559,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>23</v>
       </c>
@@ -3619,7 +3604,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -3664,7 +3649,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>25</v>
       </c>
@@ -3709,7 +3694,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>26</v>
       </c>
@@ -3754,7 +3739,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
@@ -3799,7 +3784,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>28</v>
       </c>
@@ -3844,7 +3829,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
@@ -3889,7 +3874,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
@@ -3934,7 +3919,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
@@ -3979,7 +3964,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
@@ -4024,7 +4009,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>33</v>
       </c>
@@ -4069,7 +4054,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="23.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>34</v>
       </c>
@@ -4115,7 +4100,7 @@
       </c>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>35</v>
       </c>
@@ -4161,7 +4146,7 @@
       </c>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>36</v>
       </c>
@@ -4207,7 +4192,7 @@
       </c>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>37</v>
       </c>
@@ -4253,7 +4238,7 @@
       </c>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>38</v>
       </c>
@@ -4299,7 +4284,7 @@
       </c>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>39</v>
       </c>
@@ -4345,7 +4330,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>40</v>
       </c>
@@ -4391,7 +4376,7 @@
       </c>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>41</v>
       </c>
@@ -4437,7 +4422,7 @@
       </c>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>42</v>
       </c>
@@ -4483,7 +4468,7 @@
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>43</v>
       </c>
@@ -4528,7 +4513,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
@@ -4573,7 +4558,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>45</v>
       </c>
@@ -4618,7 +4603,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
@@ -4663,7 +4648,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>47</v>
       </c>
@@ -4708,7 +4693,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>48</v>
       </c>
@@ -4753,7 +4738,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>49</v>
       </c>
@@ -4798,7 +4783,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>50</v>
       </c>
@@ -4843,7 +4828,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>51</v>
       </c>
@@ -4888,7 +4873,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <f>SUBTOTAL(103,Über112['#])</f>
         <v>45</v>
@@ -4951,43 +4936,43 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:M6"/>
+      <selection pane="bottomRight" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.5" customWidth="1"/>
-    <col min="4" max="4" width="111.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.44140625" customWidth="1"/>
+    <col min="4" max="4" width="111.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="93.6640625" customWidth="1"/>
-    <col min="8" max="8" width="49.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.5" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="69" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="160.5" customWidth="1"/>
-    <col min="21" max="21" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="93.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="93.1640625" customWidth="1"/>
-    <col min="26" max="26" width="25.5" customWidth="1"/>
-    <col min="27" max="27" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="160.44140625" customWidth="1"/>
+    <col min="21" max="21" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="93.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="93.109375" customWidth="1"/>
+    <col min="26" max="26" width="25.44140625" customWidth="1"/>
+    <col min="27" max="27" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>122</v>
       </c>
@@ -5082,7 +5067,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>1</v>
       </c>
@@ -5151,7 +5136,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -5211,7 +5196,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>1</v>
       </c>
@@ -5271,7 +5256,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <v>1</v>
       </c>
@@ -5338,7 +5323,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <v>1</v>
       </c>
@@ -5352,43 +5337,35 @@
         <v>184</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>397</v>
+        <v>91</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>397</v>
+        <v>185</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>403</v>
-      </c>
-      <c r="I6" s="31" t="s">
         <v>401</v>
       </c>
+      <c r="I6" s="31"/>
       <c r="J6" s="31" t="s">
         <v>86</v>
       </c>
       <c r="K6" s="31">
         <v>2021</v>
       </c>
-      <c r="L6" s="31" t="s">
-        <v>186</v>
-      </c>
+      <c r="L6" s="31"/>
       <c r="M6" s="31" t="s">
-        <v>400</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>160</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="N6" s="25"/>
       <c r="O6" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25" t="s">
         <v>366</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>367</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5397,7 +5374,7 @@
         <v>188</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W6" s="25" t="s">
         <v>189</v>
@@ -5418,7 +5395,7 @@
       <c r="AC6" s="25"/>
       <c r="AD6" s="25"/>
     </row>
-    <row r="7" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <v>1</v>
       </c>
@@ -5486,7 +5463,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <v>1</v>
       </c>
@@ -5549,7 +5526,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
         <v>1</v>
       </c>
@@ -5566,13 +5543,13 @@
         <v>91</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>387</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>388</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5601,7 +5578,7 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>163</v>
@@ -5614,32 +5591,31 @@
       <c r="AC9" s="25"/>
       <c r="AD9" s="25"/>
     </row>
-    <row r="10" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <v>0</v>
       </c>
       <c r="B10" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="D10" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>395</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>177</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>392</v>
-      </c>
-      <c r="I10" s="40"/>
       <c r="J10" s="25" t="s">
         <v>86</v>
       </c>
@@ -5658,19 +5634,19 @@
       </c>
       <c r="P10" s="25"/>
       <c r="Q10" s="31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="V10" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="W10" s="25" t="s">
         <v>393</v>
-      </c>
-      <c r="W10" s="25" t="s">
-        <v>394</v>
       </c>
       <c r="X10" s="25" t="s">
         <v>101</v>
@@ -5684,7 +5660,7 @@
       <c r="AC10" s="25"/>
       <c r="AD10" s="25"/>
     </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="25">
         <v>1</v>
       </c>
@@ -5751,7 +5727,7 @@
       <c r="AC11" s="25"/>
       <c r="AD11" s="25"/>
     </row>
-    <row r="12" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -5804,7 +5780,7 @@
         <v>216</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W12" s="35" t="s">
         <v>217</v>
@@ -5822,7 +5798,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <v>1</v>
       </c>
@@ -5884,7 +5860,7 @@
       <c r="AC13"/>
       <c r="AD13"/>
     </row>
-    <row r="14" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <v>1</v>
       </c>
@@ -5898,16 +5874,16 @@
         <v>225</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F14" s="25" t="s">
         <v>185</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>86</v>
@@ -5934,7 +5910,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <v>1</v>
       </c>
@@ -5945,7 +5921,7 @@
         <v>229</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
@@ -5997,7 +5973,7 @@
       <c r="AC15"/>
       <c r="AD15"/>
     </row>
-    <row r="16" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <v>1</v>
       </c>
@@ -6041,7 +6017,7 @@
         <v>241</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
@@ -6060,7 +6036,7 @@
       <c r="AC16"/>
       <c r="AD16"/>
     </row>
-    <row r="17" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" s="25" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
         <v>1</v>
       </c>
@@ -6098,7 +6074,7 @@
         <v>247</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
@@ -6114,7 +6090,7 @@
       <c r="AC17"/>
       <c r="AD17"/>
     </row>
-    <row r="18" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <v>1</v>
       </c>
@@ -6171,7 +6147,7 @@
       <c r="AC18"/>
       <c r="AD18"/>
     </row>
-    <row r="19" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <v>1</v>
       </c>
@@ -6194,7 +6170,7 @@
         <v>168</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6229,7 +6205,7 @@
       <c r="AC19"/>
       <c r="AD19"/>
     </row>
-    <row r="20" spans="1:31" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" s="25" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <v>1</v>
       </c>
@@ -6237,10 +6213,10 @@
         <v>84</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>91</v>
@@ -6252,7 +6228,7 @@
         <v>168</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6276,7 +6252,7 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W20" s="35" t="s">
         <v>263</v>
@@ -6294,7 +6270,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>1</v>
       </c>
@@ -6362,7 +6338,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>1</v>
       </c>
@@ -6421,7 +6397,7 @@
       <c r="AC22" s="25"/>
       <c r="AD22" s="25"/>
     </row>
-    <row r="23" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
         <v>1</v>
       </c>
@@ -6477,7 +6453,7 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W23" s="35" t="s">
         <v>280</v>
@@ -6495,7 +6471,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <v>1</v>
       </c>
@@ -6552,7 +6528,7 @@
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W24" s="35" t="s">
         <v>287</v>
@@ -6573,7 +6549,7 @@
       <c r="AC24" s="25"/>
       <c r="AD24" s="25"/>
     </row>
-    <row r="25" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="25">
         <v>1</v>
       </c>
@@ -6581,7 +6557,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>289</v>
@@ -6624,19 +6600,19 @@
         <v>292</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S25" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="T25" s="25" t="s">
         <v>373</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>374</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W25" s="35" t="s">
         <v>293</v>
@@ -6657,7 +6633,7 @@
       <c r="AC25" s="25"/>
       <c r="AD25" s="25"/>
     </row>
-    <row r="26" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <v>1</v>
       </c>
@@ -6720,7 +6696,7 @@
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W26" s="35" t="s">
         <v>287</v>
@@ -6741,7 +6717,7 @@
       <c r="AC26" s="25"/>
       <c r="AD26" s="25"/>
     </row>
-    <row r="27" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A27" s="25">
         <v>1</v>
       </c>
@@ -6749,7 +6725,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>300</v>
@@ -6795,16 +6771,16 @@
         <v>298</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U27" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="W27" s="35" t="s">
         <v>287</v>
@@ -6825,7 +6801,7 @@
       <c r="AC27" s="25"/>
       <c r="AD27" s="25"/>
     </row>
-    <row r="28" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="25">
         <v>1</v>
       </c>
@@ -6898,7 +6874,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <v>1</v>
       </c>
@@ -6971,7 +6947,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <v>0</v>
       </c>
@@ -7038,7 +7014,7 @@
       <c r="AD30" s="25"/>
       <c r="AE30" s="25"/>
     </row>
-    <row r="31" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <v>1</v>
       </c>
@@ -7109,7 +7085,7 @@
       <c r="AD31" s="25"/>
       <c r="AE31" s="25"/>
     </row>
-    <row r="32" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="25">
         <v>1</v>
       </c>
@@ -7132,7 +7108,7 @@
         <v>104</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7145,13 +7121,13 @@
         <v>186</v>
       </c>
       <c r="M32" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N32" s="25" t="s">
         <v>160</v>
       </c>
       <c r="O32" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P32" s="25">
         <v>1</v>
@@ -7178,7 +7154,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="25">
         <v>1</v>
       </c>
@@ -7238,7 +7214,7 @@
       <c r="AC33" s="25"/>
       <c r="AD33" s="25"/>
     </row>
-    <row r="34" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="25">
         <v>1</v>
       </c>
@@ -7291,7 +7267,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A35" s="25">
         <v>1</v>
       </c>
@@ -7362,7 +7338,7 @@
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
     </row>
-    <row r="36" spans="1:31" s="28" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" s="28" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="A36" s="25">
         <v>1</v>
       </c>
@@ -7415,7 +7391,7 @@
         <v>108</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="W36" s="25"/>
       <c r="X36" s="25" t="s">
@@ -7433,7 +7409,7 @@
       <c r="AD36" s="25"/>
       <c r="AE36" s="25"/>
     </row>
-    <row r="37" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25">
         <v>1</v>
       </c>
@@ -7486,7 +7462,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A38" s="25">
         <v>1</v>
       </c>
@@ -7552,7 +7528,7 @@
       <c r="AC38" s="25"/>
       <c r="AD38" s="25"/>
     </row>
-    <row r="39" spans="1:31" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" ht="14" x14ac:dyDescent="0.3">
       <c r="A39" s="25">
         <v>1</v>
       </c>
@@ -7618,7 +7594,7 @@
       <c r="AC39" s="25"/>
       <c r="AD39" s="25"/>
     </row>
-    <row r="40" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="25">
         <v>1</v>
       </c>
@@ -7720,6 +7696,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004D6EF8296678614C82595E073A935E63" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2c357ece3d19c143a9e4a1e033fa04b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7c16c412-41a7-483e-8458-9b4c6e041c8c" xmlns:ns3="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78066d3103febb3f607343910020d0d2" ns2:_="" ns3:_="">
     <xsd:import namespace="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
@@ -7924,27 +7920,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c16c412-41a7-483e-8458-9b4c6e041c8c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E89199-B92A-4346-AA14-A4573F72AE71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7963,31 +7964,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4E4C368-1DF5-422B-BD39-8846CE2351EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A314DA-0F62-4E10-94F7-DBFCC9F3B707}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7c16c412-41a7-483e-8458-9b4c6e041c8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9ff67bf8-4dc4-49ec-8a2f-3c58a02da8ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{ab6d1c10-a186-47ab-af91-cdbff51004f3}" enabled="1" method="Standard" siteId="{a020d0ae-094a-4d44-b66c-ac3fe8e90c58}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
LF1: longer time series
</commit_message>
<xml_diff>
--- a/2773 Monitoring.xlsx
+++ b/2773 Monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitrepos\decarb_monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D8807A-04B0-4D87-BDB7-B3D56C1BE76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1652F6D6-0A7A-4800-8E1B-91744E463733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1845" windowWidth="29040" windowHeight="17520" tabRatio="775" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1160,9 +1160,6 @@
     <t>Ständige Wohnbevölkerung</t>
   </si>
   <si>
-    <t>Ständige und nichtständige Wohnbevölkerung</t>
-  </si>
-  <si>
     <t>Personen</t>
   </si>
   <si>
@@ -1398,6 +1395,9 @@
   </si>
   <si>
     <t>1981-2010 Statistik des jährlichen Bevölkerungsstandes (ESPOP), ab 2011 Statistik der Bevölkerung und der Haushalte (STATPOP)</t>
+  </si>
+  <si>
+    <t>Demografische Bilanz nach institutionellen Gliederungen</t>
   </si>
 </sst>
 </file>
@@ -5032,10 +5032,10 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X33" sqref="X33"/>
+      <selection pane="bottomRight" activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5363,7 +5363,7 @@
         <v>113</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>91</v>
@@ -5439,10 +5439,10 @@
         <v>181</v>
       </c>
       <c r="G6" s="37" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>391</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>392</v>
       </c>
       <c r="I6" s="31"/>
       <c r="J6" s="31" t="s">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="L6" s="31"/>
       <c r="M6" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N6" s="25" t="s">
         <v>156</v>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R6" s="25"/>
       <c r="S6" s="25"/>
@@ -5472,7 +5472,7 @@
         <v>184</v>
       </c>
       <c r="V6" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="W6" s="25" t="s">
         <v>185</v>
@@ -5641,13 +5641,13 @@
         <v>91</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>377</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="H9" s="25" t="s">
         <v>378</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>379</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>86</v>
@@ -5676,7 +5676,7 @@
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Y9" s="25" t="s">
         <v>159</v>
@@ -5694,13 +5694,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>382</v>
-      </c>
       <c r="D10" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>91</v>
@@ -5712,7 +5712,7 @@
         <v>173</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>86</v>
@@ -5732,19 +5732,19 @@
       </c>
       <c r="P10" s="25"/>
       <c r="Q10" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
       <c r="U10" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="V10" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="W10" s="25" t="s">
         <v>384</v>
-      </c>
-      <c r="W10" s="25" t="s">
-        <v>385</v>
       </c>
       <c r="X10" s="25" t="s">
         <v>99</v>
@@ -5845,10 +5845,10 @@
         <v>181</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>86</v>
@@ -5857,7 +5857,7 @@
         <v>2005</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N12" s="25" t="s">
         <v>156</v>
@@ -5875,7 +5875,7 @@
         <v>212</v>
       </c>
       <c r="V12" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W12" s="35" t="s">
         <v>213</v>
@@ -5935,7 +5935,7 @@
         <v>218</v>
       </c>
       <c r="U13" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="V13" s="25" t="s">
         <v>219</v>
@@ -5969,16 +5969,16 @@
         <v>221</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F14" s="25" t="s">
         <v>181</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>86</v>
@@ -5990,7 +5990,7 @@
         <v>85</v>
       </c>
       <c r="U14" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="V14" s="25" t="s">
         <v>222</v>
@@ -6016,7 +6016,7 @@
         <v>225</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>91</v>
@@ -6112,7 +6112,7 @@
         <v>237</v>
       </c>
       <c r="V16" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="W16"/>
       <c r="X16" s="25" t="s">
@@ -6139,10 +6139,10 @@
         <v>81</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>348</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>349</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>91</v>
@@ -6169,7 +6169,7 @@
         <v>243</v>
       </c>
       <c r="V17" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="W17"/>
       <c r="X17" s="25" t="s">
@@ -6265,7 +6265,7 @@
         <v>164</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>86</v>
@@ -6308,10 +6308,10 @@
         <v>84</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>91</v>
@@ -6323,7 +6323,7 @@
         <v>164</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>86</v>
@@ -6347,7 +6347,7 @@
         <v>93</v>
       </c>
       <c r="V20" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W20" s="35" t="s">
         <v>259</v>
@@ -6512,10 +6512,10 @@
         <v>181</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>86</v>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N23" s="25" t="s">
         <v>156</v>
@@ -6546,7 +6546,7 @@
         <v>93</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W23" s="35" t="s">
         <v>276</v>
@@ -6584,10 +6584,10 @@
         <v>181</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25" t="s">
@@ -6598,7 +6598,7 @@
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N24" s="25" t="s">
         <v>156</v>
@@ -6619,7 +6619,7 @@
         <v>93</v>
       </c>
       <c r="V24" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W24" s="35" t="s">
         <v>283</v>
@@ -6648,7 +6648,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>285</v>
@@ -6660,10 +6660,10 @@
         <v>181</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I25" s="25"/>
       <c r="J25" s="25" t="s">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N25" s="25" t="s">
         <v>156</v>
@@ -6689,19 +6689,19 @@
         <v>287</v>
       </c>
       <c r="R25" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S25" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="T25" s="25" t="s">
         <v>364</v>
-      </c>
-      <c r="T25" s="25" t="s">
-        <v>365</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V25" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W25" s="35" t="s">
         <v>288</v>
@@ -6742,10 +6742,10 @@
         <v>181</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31" t="s">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="L26" s="31"/>
       <c r="M26" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N26" s="25" t="s">
         <v>156</v>
@@ -6783,7 +6783,7 @@
         <v>93</v>
       </c>
       <c r="V26" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W26" s="35" t="s">
         <v>283</v>
@@ -6812,7 +6812,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>295</v>
@@ -6824,10 +6824,10 @@
         <v>181</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="25" t="s">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="N27" s="25" t="s">
         <v>156</v>
@@ -6856,16 +6856,16 @@
         <v>293</v>
       </c>
       <c r="S27" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="T27" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="U27" s="25" t="s">
         <v>93</v>
       </c>
       <c r="V27" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="W27" s="35" t="s">
         <v>283</v>
@@ -7193,7 +7193,7 @@
         <v>102</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25" t="s">
@@ -7212,25 +7212,25 @@
         <v>156</v>
       </c>
       <c r="O32" s="25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="P32" s="25">
         <v>16</v>
       </c>
       <c r="Q32" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
       <c r="T32" s="25"/>
       <c r="U32" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="V32" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="V32" s="25" t="s">
-        <v>325</v>
-      </c>
       <c r="X32" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Y32" s="25" t="s">
         <v>159</v>
@@ -7247,10 +7247,10 @@
         <v>307</v>
       </c>
       <c r="C33" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>326</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>327</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>91</v>
@@ -7262,7 +7262,7 @@
         <v>298</v>
       </c>
       <c r="H33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I33" s="25"/>
       <c r="J33" s="25" t="s">
@@ -7307,10 +7307,10 @@
         <v>69</v>
       </c>
       <c r="C34" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="D34" s="25" t="s">
         <v>329</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>330</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>91</v>
@@ -7322,7 +7322,7 @@
         <v>173</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>86</v>
@@ -7334,7 +7334,7 @@
         <v>85</v>
       </c>
       <c r="O34" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U34" s="25" t="s">
         <v>87</v>
@@ -7343,7 +7343,7 @@
         <v>272</v>
       </c>
       <c r="X34" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Y34" s="25" t="s">
         <v>159</v>
@@ -7363,7 +7363,7 @@
         <v>308</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>91</v>
@@ -7375,7 +7375,7 @@
         <v>311</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I35" s="25"/>
       <c r="J35" s="25" t="s">
@@ -7446,7 +7446,7 @@
         <v>173</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I36" s="25"/>
       <c r="J36" s="25" t="s">
@@ -7463,11 +7463,11 @@
         <v>174</v>
       </c>
       <c r="O36" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P36" s="25"/>
       <c r="Q36" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
@@ -7476,11 +7476,11 @@
         <v>105</v>
       </c>
       <c r="V36" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="W36" s="25"/>
       <c r="X36" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y36" s="25" t="s">
         <v>207</v>
@@ -7517,7 +7517,7 @@
         <v>173</v>
       </c>
       <c r="H37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J37" t="s">
         <v>86</v>
@@ -7529,7 +7529,7 @@
         <v>85</v>
       </c>
       <c r="O37" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="U37" t="s">
         <v>87</v>
@@ -7552,13 +7552,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>149</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>151</v>
@@ -7573,7 +7573,7 @@
         <v>154</v>
       </c>
       <c r="I38" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>86</v>
@@ -7618,13 +7618,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>149</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>151</v>
@@ -7639,7 +7639,7 @@
         <v>154</v>
       </c>
       <c r="I39" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>86</v>
@@ -7684,25 +7684,25 @@
         <v>1</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G40" t="s">
         <v>173</v>
       </c>
       <c r="H40" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J40" t="s">
         <v>86</v>
@@ -7717,10 +7717,10 @@
         <v>93</v>
       </c>
       <c r="V40" t="s">
+        <v>354</v>
+      </c>
+      <c r="X40" t="s">
         <v>355</v>
-      </c>
-      <c r="X40" t="s">
-        <v>356</v>
       </c>
       <c r="Y40" t="s">
         <v>159</v>

</xml_diff>